<commit_message>
S1_E2E Data alignment and script fixing (till TC109)
</commit_message>
<xml_diff>
--- a/Excel Files/Scenario 12/S12_TestCases_Data.xlsx
+++ b/Excel Files/Scenario 12/S12_TestCases_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nasin\git\tb-ttap-brivge-v2\Excel Files\Scenario 12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5785D004-3BC7-450A-9148-BF055B203495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3FA8F9-BCFC-4766-A1B5-35D08BCBE0F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="621" firstSheet="9" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="621" firstSheet="21" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AutoIncrement" sheetId="5" r:id="rId1"/>
@@ -4000,8 +4000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF233ECF-E9BE-4D6E-8DC6-0D5B67DB1A0A}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B7:B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4341,11 +4341,11 @@
       </c>
       <c r="B2" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY())+2, DAY(TODAY())), "dd MMM yyyy")</f>
-        <v>30 Dec 2023</v>
+        <v>01 Jan 2024</v>
       </c>
       <c r="C2" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY())+3, DAY(TODAY())), "dd MMM yyyy")</f>
-        <v>30 Jan 2024</v>
+        <v>01 Feb 2024</v>
       </c>
     </row>
   </sheetData>
@@ -4358,7 +4358,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4450,11 +4450,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEB9BE66-0588-4DEC-A77E-FB3B190C02C0}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8:G8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="20.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -4470,7 +4473,7 @@
       </c>
       <c r="B2" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY())+2, DAY(TODAY())+10), "dd MMM yyyy")</f>
-        <v>09 Jan 2024</v>
+        <v>11 Jan 2024</v>
       </c>
     </row>
   </sheetData>
@@ -4509,11 +4512,11 @@
       </c>
       <c r="B2" t="str">
         <f ca="1">"c" &amp; AutoIncrement!B2&amp;AutoIncrement!A2&amp;"-23"&amp;TEXT(TODAY(),"mm")&amp;"001"</f>
-        <v>cEA05-2310001</v>
+        <v>cEA05-2311001</v>
       </c>
       <c r="C2" t="str">
         <f ca="1">"c" &amp; AutoIncrement!B2&amp;AutoIncrement!A2&amp;"-23"&amp;TEXT(TODAY(),"mm")&amp;"002"</f>
-        <v>cEA05-2310002</v>
+        <v>cEA05-2311002</v>
       </c>
     </row>
   </sheetData>
@@ -4587,11 +4590,11 @@
       </c>
       <c r="B2" t="str">
         <f ca="1">"s" &amp; AutoIncrement!B2&amp;AutoIncrement!A2&amp;"-23"&amp;TEXT(TODAY(),"mm")&amp;"001"</f>
-        <v>sEA05-2310001</v>
+        <v>sEA05-2311001</v>
       </c>
       <c r="C2" t="str">
         <f ca="1">"s" &amp; AutoIncrement!B2&amp;AutoIncrement!A2&amp;"-23"&amp;TEXT(TODAY(),"mm")&amp;"002"</f>
-        <v>sEA05-2310002</v>
+        <v>sEA05-2311002</v>
       </c>
     </row>
   </sheetData>
@@ -4630,11 +4633,11 @@
       </c>
       <c r="B2" t="str">
         <f ca="1">"p" &amp; AutoIncrement!C2&amp;AutoIncrement!A2&amp;"-23"&amp;TEXT(TODAY(),"mm")&amp;"001"</f>
-        <v>pEAs05-2310001</v>
+        <v>pEAs05-2311001</v>
       </c>
       <c r="C2" t="str">
         <f ca="1">"p" &amp; AutoIncrement!C2&amp;AutoIncrement!A2&amp;"-23"&amp;TEXT(TODAY(),"mm")&amp;"002"</f>
-        <v>pEAs05-2310002</v>
+        <v>pEAs05-2311002</v>
       </c>
     </row>
   </sheetData>
@@ -4673,11 +4676,11 @@
       </c>
       <c r="B2" t="str">
         <f ca="1">"s" &amp; AutoIncrement!C2&amp;AutoIncrement!A2&amp;"-23"&amp;TEXT(TODAY(),"mm")&amp;"001"</f>
-        <v>sEAs05-2310001</v>
+        <v>sEAs05-2311001</v>
       </c>
       <c r="C2" t="str">
         <f ca="1">"s" &amp; AutoIncrement!C2&amp;AutoIncrement!A2&amp;"-23"&amp;TEXT(TODAY(),"mm")&amp;"002"</f>
-        <v>sEAs05-2310002</v>
+        <v>sEAs05-2311002</v>
       </c>
     </row>
   </sheetData>
@@ -4788,7 +4791,7 @@
     <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="str">
         <f ca="1">'TC16-Supplier SO'!B2</f>
-        <v>sEAs05-2310001</v>
+        <v>sEAs05-2311001</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>164</v>
@@ -4805,7 +4808,7 @@
       <c r="H2" s="13"/>
       <c r="I2" s="13" t="str">
         <f ca="1">'TC15-BU PO'!B2</f>
-        <v>pEAs05-2310001</v>
+        <v>pEAs05-2311001</v>
       </c>
       <c r="J2" t="s">
         <v>36</v>
@@ -4869,7 +4872,7 @@
       <c r="H3" s="13"/>
       <c r="I3" s="13" t="str">
         <f ca="1">'TC15-BU PO'!B2</f>
-        <v>pEAs05-2310001</v>
+        <v>pEAs05-2311001</v>
       </c>
       <c r="J3" t="s">
         <v>36</v>
@@ -4935,7 +4938,7 @@
       <c r="H4" s="13"/>
       <c r="I4" s="13" t="str">
         <f ca="1">'TC15-BU PO'!B2</f>
-        <v>pEAs05-2310001</v>
+        <v>pEAs05-2311001</v>
       </c>
       <c r="J4" t="s">
         <v>36</v>
@@ -4995,7 +4998,7 @@
       </c>
       <c r="I5" s="13" t="str">
         <f ca="1">'TC15-BU PO'!B2</f>
-        <v>pEAs05-2310001</v>
+        <v>pEAs05-2311001</v>
       </c>
       <c r="J5" t="s">
         <v>36</v>
@@ -5055,7 +5058,7 @@
       </c>
       <c r="I6" s="13" t="str">
         <f ca="1">'TC15-BU PO'!B2</f>
-        <v>pEAs05-2310001</v>
+        <v>pEAs05-2311001</v>
       </c>
       <c r="J6" t="s">
         <v>36</v>
@@ -5115,7 +5118,7 @@
       </c>
       <c r="I7" s="13" t="str">
         <f ca="1">'TC15-BU PO'!B2</f>
-        <v>pEAs05-2310001</v>
+        <v>pEAs05-2311001</v>
       </c>
       <c r="J7" t="s">
         <v>36</v>
@@ -5463,7 +5466,7 @@
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="str">
         <f ca="1">'TC16-Supplier SO'!C2</f>
-        <v>sEAs05-2310002</v>
+        <v>sEAs05-2311002</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>164</v>
@@ -5476,7 +5479,7 @@
       </c>
       <c r="I2" s="13" t="str">
         <f ca="1">'TC15-BU PO'!C2</f>
-        <v>pEAs05-2310002</v>
+        <v>pEAs05-2311002</v>
       </c>
       <c r="J2" t="s">
         <v>36</v>
@@ -5527,7 +5530,7 @@
       </c>
       <c r="I3" s="13" t="str">
         <f ca="1">'TC15-BU PO'!C2</f>
-        <v>pEAs05-2310002</v>
+        <v>pEAs05-2311002</v>
       </c>
       <c r="J3" t="s">
         <v>36</v>
@@ -5578,7 +5581,7 @@
       </c>
       <c r="I4" s="13" t="str">
         <f ca="1">'TC15-BU PO'!C2</f>
-        <v>pEAs05-2310002</v>
+        <v>pEAs05-2311002</v>
       </c>
       <c r="J4" t="s">
         <v>36</v>
@@ -5629,7 +5632,7 @@
       </c>
       <c r="I5" s="13" t="str">
         <f ca="1">'TC15-BU PO'!C2</f>
-        <v>pEAs05-2310002</v>
+        <v>pEAs05-2311002</v>
       </c>
       <c r="J5" t="s">
         <v>36</v>
@@ -5680,7 +5683,7 @@
       </c>
       <c r="I6" s="13" t="str">
         <f ca="1">'TC15-BU PO'!C2</f>
-        <v>pEAs05-2310002</v>
+        <v>pEAs05-2311002</v>
       </c>
       <c r="J6" t="s">
         <v>36</v>
@@ -5731,7 +5734,7 @@
       </c>
       <c r="I7" s="13" t="str">
         <f ca="1">'TC15-BU PO'!C2</f>
-        <v>pEAs05-2310002</v>
+        <v>pEAs05-2311002</v>
       </c>
       <c r="J7" t="s">
         <v>36</v>
@@ -5820,7 +5823,7 @@
       </c>
       <c r="D2" s="1" t="str">
         <f ca="1">"rc"&amp;AutoIncrement!B2&amp;AutoIncrement!A2&amp;"-23"&amp;TEXT(TODAY(),"mm")&amp;"001-01"</f>
-        <v>rcEA05-2310001-01</v>
+        <v>rcEA05-2311001-01</v>
       </c>
       <c r="E2" t="s">
         <v>374</v>
@@ -6293,7 +6296,7 @@
       </c>
       <c r="D2" s="1" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sEA05-2310001</v>
+        <v>sEA05-2311001</v>
       </c>
       <c r="E2" t="s">
         <v>83</v>
@@ -6321,7 +6324,7 @@
       </c>
       <c r="D3" s="1" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sEA05-2310001</v>
+        <v>sEA05-2311001</v>
       </c>
       <c r="E3" t="s">
         <v>83</v>
@@ -6349,7 +6352,7 @@
       </c>
       <c r="D4" s="1" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sEA05-2310001</v>
+        <v>sEA05-2311001</v>
       </c>
       <c r="E4" t="s">
         <v>83</v>
@@ -6377,7 +6380,7 @@
       </c>
       <c r="D5" s="1" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sEA05-2310001</v>
+        <v>sEA05-2311001</v>
       </c>
       <c r="E5" t="s">
         <v>83</v>
@@ -6405,7 +6408,7 @@
       </c>
       <c r="D6" s="1" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sEA05-2310001</v>
+        <v>sEA05-2311001</v>
       </c>
       <c r="E6" t="s">
         <v>83</v>
@@ -6433,7 +6436,7 @@
       </c>
       <c r="D7" s="1" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sEA05-2310001</v>
+        <v>sEA05-2311001</v>
       </c>
       <c r="E7" t="s">
         <v>83</v>
@@ -6506,7 +6509,7 @@
       </c>
       <c r="D2" s="1" t="str">
         <f ca="1">'TC11-Customer CO'!B2</f>
-        <v>cEA05-2310001</v>
+        <v>cEA05-2311001</v>
       </c>
       <c r="E2" t="s">
         <v>36</v>
@@ -6533,7 +6536,7 @@
       </c>
       <c r="D3" s="1" t="str">
         <f ca="1">'TC11-Customer CO'!B2</f>
-        <v>cEA05-2310001</v>
+        <v>cEA05-2311001</v>
       </c>
       <c r="E3" t="s">
         <v>36</v>
@@ -6560,7 +6563,7 @@
       </c>
       <c r="D4" s="1" t="str">
         <f ca="1">'TC11-Customer CO'!B2</f>
-        <v>cEA05-2310001</v>
+        <v>cEA05-2311001</v>
       </c>
       <c r="E4" t="s">
         <v>36</v>
@@ -6587,7 +6590,7 @@
       </c>
       <c r="D5" s="1" t="str">
         <f ca="1">'TC11-Customer CO'!B2</f>
-        <v>cEA05-2310001</v>
+        <v>cEA05-2311001</v>
       </c>
       <c r="E5" t="s">
         <v>36</v>
@@ -6614,7 +6617,7 @@
       </c>
       <c r="D6" s="1" t="str">
         <f ca="1">'TC11-Customer CO'!B2</f>
-        <v>cEA05-2310001</v>
+        <v>cEA05-2311001</v>
       </c>
       <c r="E6" t="s">
         <v>36</v>
@@ -6641,7 +6644,7 @@
       </c>
       <c r="D7" s="1" t="str">
         <f ca="1">'TC11-Customer CO'!B2</f>
-        <v>cEA05-2310001</v>
+        <v>cEA05-2311001</v>
       </c>
       <c r="E7" t="s">
         <v>36</v>
@@ -6711,7 +6714,7 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sEA05-2310001</v>
+        <v>sEA05-2311001</v>
       </c>
       <c r="E2" t="s">
         <v>83</v>
@@ -6736,7 +6739,7 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sEA05-2310001</v>
+        <v>sEA05-2311001</v>
       </c>
       <c r="E3" t="s">
         <v>83</v>
@@ -6761,7 +6764,7 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sEA05-2310001</v>
+        <v>sEA05-2311001</v>
       </c>
       <c r="E4" t="s">
         <v>83</v>
@@ -6786,7 +6789,7 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sEA05-2310001</v>
+        <v>sEA05-2311001</v>
       </c>
       <c r="E5" t="s">
         <v>83</v>
@@ -6811,7 +6814,7 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sEA05-2310001</v>
+        <v>sEA05-2311001</v>
       </c>
       <c r="E6" t="s">
         <v>83</v>
@@ -6836,7 +6839,7 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sEA05-2310001</v>
+        <v>sEA05-2311001</v>
       </c>
       <c r="E7" t="s">
         <v>83</v>
@@ -7033,11 +7036,11 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY())+2, DAY(TODAY())), "dd MMM yyyy")</f>
-        <v>30 Dec 2023</v>
+        <v>01 Jan 2024</v>
       </c>
       <c r="B2" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY())+3, DAY(TODAY())), "dd MMM yyyy")</f>
-        <v>30 Jan 2024</v>
+        <v>01 Feb 2024</v>
       </c>
       <c r="C2" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY())+4, DAY(TODAY())), "dd MMM yyyy")</f>
@@ -7106,7 +7109,7 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f ca="1">"rc"&amp;AutoIncrement!B2&amp;AutoIncrement!A2&amp;"-23"&amp;TEXT(TODAY(),"mm")&amp;"001-02"</f>
-        <v>rcEA05-2310001-02</v>
+        <v>rcEA05-2311001-02</v>
       </c>
       <c r="B2" t="s">
         <v>357</v>
@@ -8049,7 +8052,7 @@
       </c>
       <c r="D2" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sEA05-2310001</v>
+        <v>sEA05-2311001</v>
       </c>
       <c r="E2" t="s">
         <v>83</v>
@@ -8109,7 +8112,7 @@
       </c>
       <c r="D3" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sEA05-2310001</v>
+        <v>sEA05-2311001</v>
       </c>
       <c r="E3" t="s">
         <v>83</v>
@@ -8169,7 +8172,7 @@
       </c>
       <c r="D4" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sEA05-2310001</v>
+        <v>sEA05-2311001</v>
       </c>
       <c r="E4" t="s">
         <v>83</v>
@@ -8229,7 +8232,7 @@
       </c>
       <c r="D5" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sEA05-2310001</v>
+        <v>sEA05-2311001</v>
       </c>
       <c r="E5" t="s">
         <v>83</v>
@@ -8289,7 +8292,7 @@
       </c>
       <c r="D6" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sEA05-2310001</v>
+        <v>sEA05-2311001</v>
       </c>
       <c r="E6" t="s">
         <v>83</v>
@@ -8349,7 +8352,7 @@
       </c>
       <c r="D7" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sEA05-2310001</v>
+        <v>sEA05-2311001</v>
       </c>
       <c r="E7" t="s">
         <v>83</v>
@@ -8505,7 +8508,7 @@
       </c>
       <c r="D2" t="str">
         <f ca="1">'TC11-Customer CO'!B2</f>
-        <v>cEA05-2310001</v>
+        <v>cEA05-2311001</v>
       </c>
       <c r="E2" t="s">
         <v>36</v>
@@ -8580,7 +8583,7 @@
       </c>
       <c r="D3" t="str">
         <f ca="1">'TC11-Customer CO'!B2</f>
-        <v>cEA05-2310001</v>
+        <v>cEA05-2311001</v>
       </c>
       <c r="E3" t="s">
         <v>36</v>
@@ -8655,7 +8658,7 @@
       </c>
       <c r="D4" t="str">
         <f ca="1">'TC11-Customer CO'!B2</f>
-        <v>cEA05-2310001</v>
+        <v>cEA05-2311001</v>
       </c>
       <c r="E4" t="s">
         <v>36</v>
@@ -8730,7 +8733,7 @@
       </c>
       <c r="D5" t="str">
         <f ca="1">'TC11-Customer CO'!B2</f>
-        <v>cEA05-2310001</v>
+        <v>cEA05-2311001</v>
       </c>
       <c r="E5" t="s">
         <v>36</v>
@@ -8805,7 +8808,7 @@
       </c>
       <c r="D6" t="str">
         <f ca="1">'TC11-Customer CO'!B2</f>
-        <v>cEA05-2310001</v>
+        <v>cEA05-2311001</v>
       </c>
       <c r="E6" t="s">
         <v>36</v>
@@ -8880,7 +8883,7 @@
       </c>
       <c r="D7" t="str">
         <f ca="1">'TC11-Customer CO'!B2</f>
-        <v>cEA05-2310001</v>
+        <v>cEA05-2311001</v>
       </c>
       <c r="E7" t="s">
         <v>36</v>
@@ -9040,7 +9043,7 @@
       <c r="C2" s="1"/>
       <c r="D2" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sEA05-2310001</v>
+        <v>sEA05-2311001</v>
       </c>
       <c r="E2" t="s">
         <v>83</v>
@@ -9104,7 +9107,7 @@
       <c r="C3" s="1"/>
       <c r="D3" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sEA05-2310001</v>
+        <v>sEA05-2311001</v>
       </c>
       <c r="E3" t="s">
         <v>83</v>
@@ -9168,7 +9171,7 @@
       <c r="C4" s="1"/>
       <c r="D4" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sEA05-2310001</v>
+        <v>sEA05-2311001</v>
       </c>
       <c r="E4" t="s">
         <v>83</v>
@@ -9232,7 +9235,7 @@
       <c r="C5" s="1"/>
       <c r="D5" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sEA05-2310001</v>
+        <v>sEA05-2311001</v>
       </c>
       <c r="E5" t="s">
         <v>83</v>
@@ -9296,7 +9299,7 @@
       <c r="C6" s="1"/>
       <c r="D6" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sEA05-2310001</v>
+        <v>sEA05-2311001</v>
       </c>
       <c r="E6" t="s">
         <v>83</v>
@@ -9360,7 +9363,7 @@
       <c r="C7" s="1"/>
       <c r="D7" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sEA05-2310001</v>
+        <v>sEA05-2311001</v>
       </c>
       <c r="E7" t="s">
         <v>83</v>
@@ -9510,7 +9513,7 @@
       </c>
       <c r="D2" t="str">
         <f ca="1">'TC15-BU PO'!B2</f>
-        <v>pEAs05-2310001</v>
+        <v>pEAs05-2311001</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>36</v>
@@ -9576,7 +9579,7 @@
       </c>
       <c r="D3" t="str">
         <f ca="1">'TC15-BU PO'!B2</f>
-        <v>pEAs05-2310001</v>
+        <v>pEAs05-2311001</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>36</v>
@@ -9642,7 +9645,7 @@
       </c>
       <c r="D4" t="str">
         <f ca="1">'TC15-BU PO'!B2</f>
-        <v>pEAs05-2310001</v>
+        <v>pEAs05-2311001</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>36</v>
@@ -9708,7 +9711,7 @@
       </c>
       <c r="D5" t="str">
         <f ca="1">'TC15-BU PO'!B2</f>
-        <v>pEAs05-2310001</v>
+        <v>pEAs05-2311001</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>36</v>
@@ -9774,7 +9777,7 @@
       </c>
       <c r="D6" t="str">
         <f ca="1">'TC15-BU PO'!B2</f>
-        <v>pEAs05-2310001</v>
+        <v>pEAs05-2311001</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>36</v>
@@ -9840,7 +9843,7 @@
       </c>
       <c r="D7" t="str">
         <f ca="1">'TC15-BU PO'!B2</f>
-        <v>pEAs05-2310001</v>
+        <v>pEAs05-2311001</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>36</v>
@@ -9937,15 +9940,15 @@
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY())+1, DAY(TODAY())), "dd MMM yyyy")</f>
-        <v>30 Nov 2023</v>
+        <v>01 Dec 2023</v>
       </c>
       <c r="B2" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY())+2, DAY(TODAY())), "dd MMM yyyy")</f>
-        <v>30 Dec 2023</v>
+        <v>01 Jan 2024</v>
       </c>
       <c r="C2" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY())+3, DAY(TODAY())), "dd MMM yyyy")</f>
-        <v>30 Jan 2024</v>
+        <v>01 Feb 2024</v>
       </c>
       <c r="D2" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY())+4, DAY(TODAY())), "dd MMM yyyy")</f>
@@ -10539,7 +10542,7 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f ca="1">"rs"&amp;AutoIncrement!C2&amp;AutoIncrement!A2&amp;"-23"&amp;TEXT(TODAY(),"mm")&amp;"001-01"</f>
-        <v>rsEAs05-2310001-01</v>
+        <v>rsEAs05-2311001-01</v>
       </c>
       <c r="B2" t="s">
         <v>356</v>
@@ -11955,26 +11958,26 @@
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="str">
         <f ca="1">"o-SG-BAFCO-"&amp;TEXT(TODAY(),"yymm") &amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>o-SG-BAFCO-2310-01-005</v>
+        <v>o-SG-BAFCO-2311-01-005</v>
       </c>
       <c r="B3" s="29" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY()), DAY(TODAY())-1), "dd MMM yyyy")</f>
-        <v>29 Oct 2023</v>
+        <v>31 Oct 2023</v>
       </c>
       <c r="C3" s="29" t="str">
         <f ca="1">"B-"&amp;TEXT(TODAY(),"yymm")&amp;"-"&amp;AutoIncrement!B2&amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>B-2310-EA-01-005</v>
+        <v>B-2311-EA-01-005</v>
       </c>
       <c r="D3" s="44">
         <v>1000</v>
       </c>
       <c r="E3" s="29" t="str">
         <f t="shared" ref="E3:E8" ca="1" si="0">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY()), DAY(TODAY())+2), "dd MMM yyyy")</f>
-        <v>01 Nov 2023</v>
+        <v>03 Nov 2023</v>
       </c>
       <c r="F3" s="29" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY()), DAY(TODAY())+10), "dd MMM yyyy")</f>
-        <v>09 Nov 2023</v>
+        <v>11 Nov 2023</v>
       </c>
       <c r="G3" s="31"/>
       <c r="H3" s="6"/>
@@ -11985,7 +11988,7 @@
       <c r="M3" s="32"/>
       <c r="N3" s="29" t="str">
         <f ca="1">"OP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>OP-231030-01-005</v>
+        <v>OP-231101-01-005</v>
       </c>
       <c r="O3" s="6" t="s">
         <v>241</v>
@@ -12001,7 +12004,7 @@
       </c>
       <c r="S3" s="29" t="str">
         <f ca="1">"IP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>IP-231030-01-005</v>
+        <v>IP-231101-01-005</v>
       </c>
       <c r="T3" s="33"/>
       <c r="U3" s="34">
@@ -12017,26 +12020,26 @@
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="str">
         <f ca="1">"o-SG-BAFCO-"&amp;TEXT(TODAY(),"yymm") &amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>o-SG-BAFCO-2310-01-005</v>
+        <v>o-SG-BAFCO-2311-01-005</v>
       </c>
       <c r="B4" s="29" t="str">
         <f t="shared" ref="B4:B8" ca="1" si="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY()), DAY(TODAY())-1), "dd MMM yyyy")</f>
-        <v>29 Oct 2023</v>
+        <v>31 Oct 2023</v>
       </c>
       <c r="C4" s="29" t="str">
         <f ca="1">"B-"&amp;TEXT(TODAY(),"yymm")&amp;"-"&amp;AutoIncrement!B2&amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>B-2310-EA-01-005</v>
+        <v>B-2311-EA-01-005</v>
       </c>
       <c r="D4" s="44">
         <v>800</v>
       </c>
       <c r="E4" s="29" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>01 Nov 2023</v>
+        <v>03 Nov 2023</v>
       </c>
       <c r="F4" s="29" t="str">
         <f t="shared" ref="F4:F8" ca="1" si="2">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY()), DAY(TODAY())+10), "dd MMM yyyy")</f>
-        <v>09 Nov 2023</v>
+        <v>11 Nov 2023</v>
       </c>
       <c r="G4" s="31" t="s">
         <v>259</v>
@@ -12049,7 +12052,7 @@
       <c r="M4" s="32"/>
       <c r="N4" s="29" t="str">
         <f ca="1">"OP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>OP-231030-01-005</v>
+        <v>OP-231101-01-005</v>
       </c>
       <c r="O4" s="6" t="s">
         <v>242</v>
@@ -12065,7 +12068,7 @@
       </c>
       <c r="S4" s="29" t="str">
         <f ca="1">"IP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-02-0"&amp;AutoIncrement!A2</f>
-        <v>IP-231030-02-005</v>
+        <v>IP-231101-02-005</v>
       </c>
       <c r="T4" s="33" t="s">
         <v>251</v>
@@ -12083,26 +12086,26 @@
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="30" t="str">
         <f ca="1">"o-SG-BAFCO-"&amp;TEXT(TODAY(),"yymm") &amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>o-SG-BAFCO-2310-01-005</v>
+        <v>o-SG-BAFCO-2311-01-005</v>
       </c>
       <c r="B5" s="29" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>29 Oct 2023</v>
+        <v>31 Oct 2023</v>
       </c>
       <c r="C5" s="29" t="str">
         <f ca="1">"B-"&amp;TEXT(TODAY(),"yymm")&amp;"-"&amp;AutoIncrement!B2&amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>B-2310-EA-01-005</v>
+        <v>B-2311-EA-01-005</v>
       </c>
       <c r="D5" s="44">
         <v>900</v>
       </c>
       <c r="E5" s="29" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>01 Nov 2023</v>
+        <v>03 Nov 2023</v>
       </c>
       <c r="F5" s="29" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>09 Nov 2023</v>
+        <v>11 Nov 2023</v>
       </c>
       <c r="G5" s="31" t="s">
         <v>239</v>
@@ -12125,7 +12128,7 @@
       </c>
       <c r="N5" s="29" t="str">
         <f ca="1">"OP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-02-0"&amp;AutoIncrement!A2</f>
-        <v>OP-231030-02-005</v>
+        <v>OP-231101-02-005</v>
       </c>
       <c r="O5" s="6" t="s">
         <v>242</v>
@@ -12148,26 +12151,26 @@
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="30" t="str">
         <f ca="1">"o-SG-BAFCO-"&amp;TEXT(TODAY(),"yymm") &amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>o-SG-BAFCO-2310-01-005</v>
+        <v>o-SG-BAFCO-2311-01-005</v>
       </c>
       <c r="B6" s="29" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>29 Oct 2023</v>
+        <v>31 Oct 2023</v>
       </c>
       <c r="C6" s="29" t="str">
         <f ca="1">"B-"&amp;TEXT(TODAY(),"yymm")&amp;"-"&amp;AutoIncrement!B2&amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>B-2310-EA-01-005</v>
+        <v>B-2311-EA-01-005</v>
       </c>
       <c r="D6" s="44">
         <v>1200</v>
       </c>
       <c r="E6" s="29" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>01 Nov 2023</v>
+        <v>03 Nov 2023</v>
       </c>
       <c r="F6" s="29" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>09 Nov 2023</v>
+        <v>11 Nov 2023</v>
       </c>
       <c r="G6" s="31" t="s">
         <v>239</v>
@@ -12192,7 +12195,7 @@
       </c>
       <c r="N6" s="29" t="str">
         <f ca="1">"OP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-02-0"&amp;AutoIncrement!A2</f>
-        <v>OP-231030-02-005</v>
+        <v>OP-231101-02-005</v>
       </c>
       <c r="O6" s="6" t="s">
         <v>242</v>
@@ -12215,26 +12218,26 @@
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="30" t="str">
         <f ca="1">"o-SG-BAFCO-"&amp;TEXT(TODAY(),"yymm") &amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>o-SG-BAFCO-2310-01-005</v>
+        <v>o-SG-BAFCO-2311-01-005</v>
       </c>
       <c r="B7" s="29" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>29 Oct 2023</v>
+        <v>31 Oct 2023</v>
       </c>
       <c r="C7" s="29" t="str">
         <f ca="1">"B-"&amp;TEXT(TODAY(),"yymm")&amp;"-"&amp;AutoIncrement!B2&amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>B-2310-EA-01-005</v>
+        <v>B-2311-EA-01-005</v>
       </c>
       <c r="D7" s="44">
         <v>1000</v>
       </c>
       <c r="E7" s="29" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>01 Nov 2023</v>
+        <v>03 Nov 2023</v>
       </c>
       <c r="F7" s="29" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>09 Nov 2023</v>
+        <v>11 Nov 2023</v>
       </c>
       <c r="G7" s="31" t="s">
         <v>240</v>
@@ -12259,7 +12262,7 @@
       </c>
       <c r="N7" s="29" t="str">
         <f ca="1">"OP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-03-0"&amp;AutoIncrement!A2</f>
-        <v>OP-231030-03-005</v>
+        <v>OP-231101-03-005</v>
       </c>
       <c r="O7" s="6" t="s">
         <v>243</v>
@@ -12275,7 +12278,7 @@
       </c>
       <c r="S7" s="29" t="str">
         <f ca="1">"IP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>IP-231030-01-005</v>
+        <v>IP-231101-01-005</v>
       </c>
       <c r="T7" s="33" t="s">
         <v>251</v>
@@ -12293,26 +12296,26 @@
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="30" t="str">
         <f ca="1">"o-SG-BAFCO-"&amp;TEXT(TODAY(),"yymm") &amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>o-SG-BAFCO-2310-01-005</v>
+        <v>o-SG-BAFCO-2311-01-005</v>
       </c>
       <c r="B8" s="29" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>29 Oct 2023</v>
+        <v>31 Oct 2023</v>
       </c>
       <c r="C8" s="29" t="str">
         <f ca="1">"B-"&amp;TEXT(TODAY(),"yymm")&amp;"-"&amp;AutoIncrement!B2&amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>B-2310-EA-01-005</v>
+        <v>B-2311-EA-01-005</v>
       </c>
       <c r="D8" s="44">
         <v>1100</v>
       </c>
       <c r="E8" s="29" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>01 Nov 2023</v>
+        <v>03 Nov 2023</v>
       </c>
       <c r="F8" s="29" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>09 Nov 2023</v>
+        <v>11 Nov 2023</v>
       </c>
       <c r="G8" s="31" t="s">
         <v>240</v>
@@ -12337,7 +12340,7 @@
       </c>
       <c r="N8" s="29" t="str">
         <f ca="1">"OP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-03-0"&amp;AutoIncrement!A2</f>
-        <v>OP-231030-03-005</v>
+        <v>OP-231101-03-005</v>
       </c>
       <c r="O8" s="6" t="s">
         <v>243</v>
@@ -12353,7 +12356,7 @@
       </c>
       <c r="S8" s="29" t="str">
         <f ca="1">"IP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-02-0"&amp;AutoIncrement!A2</f>
-        <v>IP-231030-02-005</v>
+        <v>IP-231101-02-005</v>
       </c>
       <c r="T8" s="33" t="s">
         <v>258</v>
@@ -12656,11 +12659,11 @@
       </c>
       <c r="C3" s="30" t="str">
         <f ca="1">"o-SG-BAFCO-"&amp;TEXT(TODAY(),"yymm") &amp; "-02-0"&amp;AutoIncrement!A2</f>
-        <v>o-SG-BAFCO-2310-02-005</v>
+        <v>o-SG-BAFCO-2311-02-005</v>
       </c>
       <c r="D3" s="29" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY()), DAY(TODAY())-1), "dd MMM yyyy")</f>
-        <v>29 Oct 2023</v>
+        <v>31 Oct 2023</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>210</v>
@@ -12685,11 +12688,11 @@
       </c>
       <c r="N3" s="29" t="str">
         <f t="shared" ref="N3:N10" ca="1" si="0">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY()), DAY(TODAY())+2), "dd MMM yyyy")</f>
-        <v>01 Nov 2023</v>
+        <v>03 Nov 2023</v>
       </c>
       <c r="O3" s="29" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY()), DAY(TODAY())+10), "dd MMM yyyy")</f>
-        <v>09 Nov 2023</v>
+        <v>11 Nov 2023</v>
       </c>
       <c r="P3" s="17" t="s">
         <v>271</v>
@@ -12702,7 +12705,7 @@
       <c r="V3" s="36"/>
       <c r="W3" s="29" t="str">
         <f ca="1">"OP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-02-0"&amp;AutoIncrement!A2</f>
-        <v>OP-231030-02-005</v>
+        <v>OP-231101-02-005</v>
       </c>
       <c r="X3" s="17" t="s">
         <v>272</v>
@@ -12712,7 +12715,7 @@
       <c r="AA3" s="36"/>
       <c r="AB3" s="29" t="str">
         <f ca="1">"IP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>IP-231030-01-005</v>
+        <v>IP-231101-01-005</v>
       </c>
       <c r="AC3" s="37" t="s">
         <v>273</v>
@@ -12722,7 +12725,7 @@
       <c r="AF3" s="36"/>
       <c r="AG3" s="29" t="str">
         <f ca="1">'TC16-Supplier SO'!C2</f>
-        <v>sEAs05-2310002</v>
+        <v>sEAs05-2311002</v>
       </c>
       <c r="AH3" s="29" t="s">
         <v>83</v>
@@ -12751,11 +12754,11 @@
       </c>
       <c r="C4" s="30" t="str">
         <f ca="1">"o-SG-BAFCO-"&amp;TEXT(TODAY(),"yymm") &amp; "-02-0"&amp;AutoIncrement!A2</f>
-        <v>o-SG-BAFCO-2310-02-005</v>
+        <v>o-SG-BAFCO-2311-02-005</v>
       </c>
       <c r="D4" s="29" t="str">
         <f t="shared" ref="D4:D10" ca="1" si="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY()), DAY(TODAY())-1), "dd MMM yyyy")</f>
-        <v>29 Oct 2023</v>
+        <v>31 Oct 2023</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>210</v>
@@ -12780,11 +12783,11 @@
       </c>
       <c r="N4" s="29" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>01 Nov 2023</v>
+        <v>03 Nov 2023</v>
       </c>
       <c r="O4" s="29" t="str">
         <f t="shared" ref="O4:O10" ca="1" si="2">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY()), DAY(TODAY())+10), "dd MMM yyyy")</f>
-        <v>09 Nov 2023</v>
+        <v>11 Nov 2023</v>
       </c>
       <c r="P4" s="17" t="s">
         <v>271</v>
@@ -12797,7 +12800,7 @@
       <c r="V4" s="36"/>
       <c r="W4" s="29" t="str">
         <f ca="1">"OP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-02-0"&amp;AutoIncrement!A2</f>
-        <v>OP-231030-02-005</v>
+        <v>OP-231101-02-005</v>
       </c>
       <c r="X4" s="17" t="s">
         <v>272</v>
@@ -12807,7 +12810,7 @@
       <c r="AA4" s="36"/>
       <c r="AB4" s="29" t="str">
         <f ca="1">"IP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-02-0"&amp;AutoIncrement!A2</f>
-        <v>IP-231030-02-005</v>
+        <v>IP-231101-02-005</v>
       </c>
       <c r="AC4" s="37" t="s">
         <v>274</v>
@@ -12817,7 +12820,7 @@
       <c r="AF4" s="36"/>
       <c r="AG4" s="29" t="str">
         <f ca="1">'TC16-Supplier SO'!C2</f>
-        <v>sEAs05-2310002</v>
+        <v>sEAs05-2311002</v>
       </c>
       <c r="AH4" s="29" t="s">
         <v>83</v>
@@ -12846,11 +12849,11 @@
       </c>
       <c r="C5" s="30" t="str">
         <f ca="1">"o-SG-BAFCO-"&amp;TEXT(TODAY(),"yymm") &amp; "-02-0"&amp;AutoIncrement!A2</f>
-        <v>o-SG-BAFCO-2310-02-005</v>
+        <v>o-SG-BAFCO-2311-02-005</v>
       </c>
       <c r="D5" s="29" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>29 Oct 2023</v>
+        <v>31 Oct 2023</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>28</v>
@@ -12875,11 +12878,11 @@
       </c>
       <c r="N5" s="29" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>01 Nov 2023</v>
+        <v>03 Nov 2023</v>
       </c>
       <c r="O5" s="29" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>09 Nov 2023</v>
+        <v>11 Nov 2023</v>
       </c>
       <c r="P5" s="31" t="s">
         <v>271</v>
@@ -12892,7 +12895,7 @@
       <c r="V5" s="32"/>
       <c r="W5" s="29" t="str">
         <f ca="1">"OP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>OP-231030-01-005</v>
+        <v>OP-231101-01-005</v>
       </c>
       <c r="X5" s="6" t="s">
         <v>275</v>
@@ -12908,7 +12911,7 @@
       </c>
       <c r="AB5" s="29" t="str">
         <f ca="1">"IP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-02-0"&amp;AutoIncrement!A2</f>
-        <v>IP-231030-02-005</v>
+        <v>IP-231101-02-005</v>
       </c>
       <c r="AC5" s="33" t="s">
         <v>276</v>
@@ -12918,7 +12921,7 @@
       <c r="AF5" s="32"/>
       <c r="AG5" s="29" t="str">
         <f ca="1">'TC16-Supplier SO'!C2</f>
-        <v>sEAs05-2310002</v>
+        <v>sEAs05-2311002</v>
       </c>
       <c r="AH5" s="29" t="s">
         <v>83</v>
@@ -12947,11 +12950,11 @@
       </c>
       <c r="C6" s="30" t="str">
         <f ca="1">"o-SG-BAFCO-"&amp;TEXT(TODAY(),"yymm") &amp; "-02-0"&amp;AutoIncrement!A2</f>
-        <v>o-SG-BAFCO-2310-02-005</v>
+        <v>o-SG-BAFCO-2311-02-005</v>
       </c>
       <c r="D6" s="29" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>29 Oct 2023</v>
+        <v>31 Oct 2023</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>29</v>
@@ -12976,11 +12979,11 @@
       </c>
       <c r="N6" s="29" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>01 Nov 2023</v>
+        <v>03 Nov 2023</v>
       </c>
       <c r="O6" s="29" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>09 Nov 2023</v>
+        <v>11 Nov 2023</v>
       </c>
       <c r="P6" s="4" t="s">
         <v>277</v>
@@ -13005,7 +13008,7 @@
       </c>
       <c r="W6" s="29" t="str">
         <f ca="1">"OP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>OP-231030-01-005</v>
+        <v>OP-231101-01-005</v>
       </c>
       <c r="X6" s="17" t="s">
         <v>281</v>
@@ -13015,7 +13018,7 @@
       <c r="AA6" s="36"/>
       <c r="AB6" s="29" t="str">
         <f ca="1">"IP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>IP-231030-01-005</v>
+        <v>IP-231101-01-005</v>
       </c>
       <c r="AC6" s="37"/>
       <c r="AD6" s="36"/>
@@ -13023,7 +13026,7 @@
       <c r="AF6" s="36"/>
       <c r="AG6" s="29" t="str">
         <f ca="1">'TC16-Supplier SO'!C2</f>
-        <v>sEAs05-2310002</v>
+        <v>sEAs05-2311002</v>
       </c>
       <c r="AH6" s="29" t="s">
         <v>83</v>
@@ -13052,15 +13055,15 @@
       </c>
       <c r="C7" s="30" t="str">
         <f ca="1">"o-SG-BAFCO-"&amp;TEXT(TODAY(),"yymm") &amp; "-03-0"&amp;AutoIncrement!A2</f>
-        <v>o-SG-BAFCO-2310-03-005</v>
+        <v>o-SG-BAFCO-2311-03-005</v>
       </c>
       <c r="D7" s="29" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>29 Oct 2023</v>
+        <v>31 Oct 2023</v>
       </c>
       <c r="F7" s="29" t="str">
         <f ca="1">"B-"&amp;TEXT(TODAY(),"yymm")&amp;"-"&amp;AutoIncrement!B2&amp; "-02-0"&amp;AutoIncrement!A2</f>
-        <v>B-2310-EA-02-005</v>
+        <v>B-2311-EA-02-005</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>30</v>
@@ -13085,11 +13088,11 @@
       </c>
       <c r="N7" s="29" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>01 Nov 2023</v>
+        <v>03 Nov 2023</v>
       </c>
       <c r="O7" s="29" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>09 Nov 2023</v>
+        <v>11 Nov 2023</v>
       </c>
       <c r="P7" s="4" t="s">
         <v>282</v>
@@ -13106,7 +13109,7 @@
       <c r="V7" s="36"/>
       <c r="W7" s="29" t="str">
         <f ca="1">"OP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>OP-231030-01-005</v>
+        <v>OP-231101-01-005</v>
       </c>
       <c r="X7" s="17" t="s">
         <v>281</v>
@@ -13121,7 +13124,7 @@
       <c r="AF7" s="36"/>
       <c r="AG7" s="29" t="str">
         <f ca="1">'TC16-Supplier SO'!C2</f>
-        <v>sEAs05-2310002</v>
+        <v>sEAs05-2311002</v>
       </c>
       <c r="AH7" s="29" t="s">
         <v>83</v>
@@ -13150,15 +13153,15 @@
       </c>
       <c r="C8" s="30" t="str">
         <f ca="1">"o-SG-BAFCO-"&amp;TEXT(TODAY(),"yymm") &amp; "-03-0"&amp;AutoIncrement!A2</f>
-        <v>o-SG-BAFCO-2310-03-005</v>
+        <v>o-SG-BAFCO-2311-03-005</v>
       </c>
       <c r="D8" s="29" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>29 Oct 2023</v>
+        <v>31 Oct 2023</v>
       </c>
       <c r="F8" s="29" t="str">
         <f ca="1">"B-"&amp;TEXT(TODAY(),"yymm")&amp;"-"&amp;AutoIncrement!B2&amp; "-02-0"&amp;AutoIncrement!A2</f>
-        <v>B-2310-EA-02-005</v>
+        <v>B-2311-EA-02-005</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>171</v>
@@ -13183,11 +13186,11 @@
       </c>
       <c r="N8" s="29" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>01 Nov 2023</v>
+        <v>03 Nov 2023</v>
       </c>
       <c r="O8" s="29" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>09 Nov 2023</v>
+        <v>11 Nov 2023</v>
       </c>
       <c r="P8" s="4" t="s">
         <v>282</v>
@@ -13204,7 +13207,7 @@
       <c r="V8" s="36"/>
       <c r="W8" s="29" t="str">
         <f ca="1">"OP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-02-0"&amp;AutoIncrement!A2</f>
-        <v>OP-231030-02-005</v>
+        <v>OP-231101-02-005</v>
       </c>
       <c r="X8" s="17" t="s">
         <v>275</v>
@@ -13219,7 +13222,7 @@
       <c r="AF8" s="36"/>
       <c r="AG8" s="29" t="str">
         <f ca="1">'TC16-Supplier SO'!C2</f>
-        <v>sEAs05-2310002</v>
+        <v>sEAs05-2311002</v>
       </c>
       <c r="AH8" s="29" t="s">
         <v>83</v>
@@ -13248,15 +13251,15 @@
       </c>
       <c r="C9" s="30" t="str">
         <f ca="1">"o-SG-BAFCO-"&amp;TEXT(TODAY(),"yymm") &amp; "-03-0"&amp;AutoIncrement!A2</f>
-        <v>o-SG-BAFCO-2310-03-005</v>
+        <v>o-SG-BAFCO-2311-03-005</v>
       </c>
       <c r="D9" s="29" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>29 Oct 2023</v>
+        <v>31 Oct 2023</v>
       </c>
       <c r="F9" s="29" t="str">
         <f ca="1">"B-"&amp;TEXT(TODAY(),"yymm")&amp;"-"&amp;AutoIncrement!B2&amp; "-02-0"&amp;AutoIncrement!A2</f>
-        <v>B-2310-EA-02-005</v>
+        <v>B-2311-EA-02-005</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>287</v>
@@ -13281,11 +13284,11 @@
       </c>
       <c r="N9" s="29" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>01 Nov 2023</v>
+        <v>03 Nov 2023</v>
       </c>
       <c r="O9" s="29" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>09 Nov 2023</v>
+        <v>11 Nov 2023</v>
       </c>
       <c r="P9" s="4" t="s">
         <v>284</v>
@@ -13310,7 +13313,7 @@
       </c>
       <c r="W9" s="29" t="str">
         <f ca="1">"OP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-03-0"&amp;AutoIncrement!A2</f>
-        <v>OP-231030-03-005</v>
+        <v>OP-231101-03-005</v>
       </c>
       <c r="X9" s="17" t="s">
         <v>275</v>
@@ -13326,7 +13329,7 @@
       </c>
       <c r="AB9" s="29" t="str">
         <f ca="1">"IP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>IP-231030-01-005</v>
+        <v>IP-231101-01-005</v>
       </c>
       <c r="AC9" s="37" t="s">
         <v>276</v>
@@ -13342,7 +13345,7 @@
       </c>
       <c r="AG9" s="29" t="str">
         <f ca="1">'TC16-Supplier SO'!C2</f>
-        <v>sEAs05-2310002</v>
+        <v>sEAs05-2311002</v>
       </c>
       <c r="AH9" s="29" t="s">
         <v>83</v>
@@ -13371,15 +13374,15 @@
       </c>
       <c r="C10" s="30" t="str">
         <f ca="1">"o-SG-BAFCO-"&amp;TEXT(TODAY(),"yymm") &amp; "-04-0"&amp;AutoIncrement!A2</f>
-        <v>o-SG-BAFCO-2310-04-005</v>
+        <v>o-SG-BAFCO-2311-04-005</v>
       </c>
       <c r="D10" s="29" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>29 Oct 2023</v>
+        <v>31 Oct 2023</v>
       </c>
       <c r="F10" s="29" t="str">
         <f ca="1">"B-"&amp;TEXT(TODAY(),"yymm")&amp;"-"&amp;AutoIncrement!B2&amp; "-03-0"&amp;AutoIncrement!A2</f>
-        <v>B-2310-EA-03-005</v>
+        <v>B-2311-EA-03-005</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>287</v>
@@ -13404,11 +13407,11 @@
       </c>
       <c r="N10" s="29" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>01 Nov 2023</v>
+        <v>03 Nov 2023</v>
       </c>
       <c r="O10" s="29" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>09 Nov 2023</v>
+        <v>11 Nov 2023</v>
       </c>
       <c r="P10" s="17"/>
       <c r="Q10" s="17"/>
@@ -13419,7 +13422,7 @@
       <c r="V10" s="36"/>
       <c r="W10" s="29" t="str">
         <f ca="1">"OP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-03-0"&amp;AutoIncrement!A2</f>
-        <v>OP-231030-03-005</v>
+        <v>OP-231101-03-005</v>
       </c>
       <c r="X10" s="17" t="s">
         <v>275</v>
@@ -13435,7 +13438,7 @@
       </c>
       <c r="AB10" s="29" t="str">
         <f ca="1">"IP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>IP-231030-01-005</v>
+        <v>IP-231101-01-005</v>
       </c>
       <c r="AC10" s="37" t="s">
         <v>276</v>
@@ -13451,7 +13454,7 @@
       </c>
       <c r="AG10" s="29" t="str">
         <f ca="1">'TC16-Supplier SO'!C2</f>
-        <v>sEAs05-2310002</v>
+        <v>sEAs05-2311002</v>
       </c>
       <c r="AH10" s="29" t="s">
         <v>83</v>
@@ -13768,7 +13771,7 @@
     <row r="2" spans="1:26" s="41" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="str">
         <f ca="1">'TC44-Supplier Outbound -Regular'!C3</f>
-        <v>B-2310-EA-01-005</v>
+        <v>B-2311-EA-01-005</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="13" t="s">
@@ -13847,7 +13850,7 @@
     <row r="3" spans="1:26" s="41" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="str">
         <f ca="1">'TC44-Supplier Outbound -Regular'!C3</f>
-        <v>B-2310-EA-01-005</v>
+        <v>B-2311-EA-01-005</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>259</v>
@@ -13928,7 +13931,7 @@
     <row r="4" spans="1:26" s="41" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="str">
         <f ca="1">'TC44-Supplier Outbound -Regular'!C3</f>
-        <v>B-2310-EA-01-005</v>
+        <v>B-2311-EA-01-005</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>345</v>
@@ -14009,7 +14012,7 @@
     <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="str">
         <f ca="1">'TC44-Supplier Outbound -Regular'!C3</f>
-        <v>B-2310-EA-01-005</v>
+        <v>B-2311-EA-01-005</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>346</v>
@@ -14213,7 +14216,7 @@
     <row r="2" spans="1:26" s="41" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="str">
         <f ca="1">'TC44-Supplier Outbound -Spot'!F7</f>
-        <v>B-2310-EA-02-005</v>
+        <v>B-2311-EA-02-005</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>346</v>
@@ -14372,7 +14375,7 @@
     <row r="4" spans="1:26" s="41" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="str">
         <f ca="1">'TC44-Supplier Outbound -Spot'!F8</f>
-        <v>B-2310-EA-02-005</v>
+        <v>B-2311-EA-02-005</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>345</v>
@@ -14453,7 +14456,7 @@
     <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="str">
         <f ca="1">'TC44-Supplier Outbound -Spot'!F10</f>
-        <v>B-2310-EA-03-005</v>
+        <v>B-2311-EA-03-005</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>342</v>
@@ -14698,13 +14701,13 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f ca="1">'TC44-Supplier Outbound -Regular'!C3</f>
-        <v>B-2310-EA-01-005</v>
+        <v>B-2311-EA-01-005</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="str">
         <f ca="1">'TC44-Supplier Outbound -Regular'!C8</f>
-        <v>B-2310-EA-01-005</v>
+        <v>B-2311-EA-01-005</v>
       </c>
       <c r="B3" s="2" t="str">
         <f>'TC44-Supplier Outbound -Regular'!G8</f>
@@ -14714,7 +14717,7 @@
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="str">
         <f ca="1">'TC44-Supplier Outbound -Regular'!C4</f>
-        <v>B-2310-EA-01-005</v>
+        <v>B-2311-EA-01-005</v>
       </c>
       <c r="B4" s="42" t="str">
         <f>'TC44-Supplier Outbound -Regular'!G4</f>
@@ -14724,7 +14727,7 @@
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="str">
         <f ca="1">'TC44-Supplier Outbound -Regular'!C6</f>
-        <v>B-2310-EA-01-005</v>
+        <v>B-2311-EA-01-005</v>
       </c>
       <c r="B5" s="42" t="str">
         <f>'TC44-Supplier Outbound -Regular'!G6</f>
@@ -14747,7 +14750,7 @@
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f ca="1">'TC44-Supplier Outbound -Spot'!F9</f>
-        <v>B-2310-EA-02-005</v>
+        <v>B-2311-EA-02-005</v>
       </c>
       <c r="B8" s="2" t="str">
         <f>'TC44-Supplier Outbound -Spot'!P9</f>
@@ -14757,7 +14760,7 @@
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f ca="1">'TC44-Supplier Outbound -Spot'!F8</f>
-        <v>B-2310-EA-02-005</v>
+        <v>B-2311-EA-02-005</v>
       </c>
       <c r="B9" s="2" t="str">
         <f>'TC44-Supplier Outbound -Spot'!P8</f>
@@ -14767,7 +14770,7 @@
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f ca="1">'TC44-Supplier Outbound -Spot'!F10</f>
-        <v>B-2310-EA-03-005</v>
+        <v>B-2311-EA-03-005</v>
       </c>
     </row>
   </sheetData>
@@ -14894,11 +14897,11 @@
       </c>
       <c r="B2" t="str">
         <f ca="1">"i-VN-AKIRA-"&amp;TEXT(TODAY(),"yymmdd") &amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>i-VN-AKIRA-231030-01-005</v>
+        <v>i-VN-AKIRA-231101-01-005</v>
       </c>
       <c r="C2" s="29" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY()), DAY(TODAY())), "dd MMM yyyy")</f>
-        <v>30 Oct 2023</v>
+        <v>01 Nov 2023</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -14907,11 +14910,11 @@
       </c>
       <c r="B3" t="str">
         <f ca="1">"i-VN-AKIRA-"&amp;TEXT(TODAY(),"yymmdd") &amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>i-VN-AKIRA-231030-01-005</v>
+        <v>i-VN-AKIRA-231101-01-005</v>
       </c>
       <c r="C3" s="29" t="str">
         <f t="shared" ref="C3:C15" ca="1" si="0">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY()), DAY(TODAY())), "dd MMM yyyy")</f>
-        <v>30 Oct 2023</v>
+        <v>01 Nov 2023</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -14920,11 +14923,11 @@
       </c>
       <c r="B4" t="str">
         <f ca="1">"i-VN-AKIRA-"&amp;TEXT(TODAY(),"yymmdd") &amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>i-VN-AKIRA-231030-01-005</v>
+        <v>i-VN-AKIRA-231101-01-005</v>
       </c>
       <c r="C4" s="29" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>30 Oct 2023</v>
+        <v>01 Nov 2023</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -14933,11 +14936,11 @@
       </c>
       <c r="B5" t="str">
         <f ca="1">"i-VN-AKIRA-"&amp;TEXT(TODAY(),"yymmdd") &amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>i-VN-AKIRA-231030-01-005</v>
+        <v>i-VN-AKIRA-231101-01-005</v>
       </c>
       <c r="C5" s="29" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>30 Oct 2023</v>
+        <v>01 Nov 2023</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -14946,11 +14949,11 @@
       </c>
       <c r="B6" t="str">
         <f ca="1">"i-VN-AKIRA-"&amp;TEXT(TODAY(),"yymmdd") &amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>i-VN-AKIRA-231030-01-005</v>
+        <v>i-VN-AKIRA-231101-01-005</v>
       </c>
       <c r="C6" s="29" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>30 Oct 2023</v>
+        <v>01 Nov 2023</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -14959,11 +14962,11 @@
       </c>
       <c r="B7" t="str">
         <f ca="1">"i-VN-AKIRA-"&amp;TEXT(TODAY(),"yymmdd") &amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>i-VN-AKIRA-231030-01-005</v>
+        <v>i-VN-AKIRA-231101-01-005</v>
       </c>
       <c r="C7" s="29" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>30 Oct 2023</v>
+        <v>01 Nov 2023</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -14972,11 +14975,11 @@
       </c>
       <c r="B8" t="str">
         <f ca="1">"i-VN-AKIRA-"&amp;TEXT(TODAY(),"yymmdd") &amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>i-VN-AKIRA-231030-01-005</v>
+        <v>i-VN-AKIRA-231101-01-005</v>
       </c>
       <c r="C8" s="29" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>30 Oct 2023</v>
+        <v>01 Nov 2023</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -14985,11 +14988,11 @@
       </c>
       <c r="B9" t="str">
         <f ca="1">"i-VN-AKIRA-"&amp;TEXT(TODAY(),"yymmdd") &amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>i-VN-AKIRA-231030-01-005</v>
+        <v>i-VN-AKIRA-231101-01-005</v>
       </c>
       <c r="C9" s="29" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>30 Oct 2023</v>
+        <v>01 Nov 2023</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -14998,11 +15001,11 @@
       </c>
       <c r="B10" t="str">
         <f ca="1">"i-VN-AKIRA-"&amp;TEXT(TODAY(),"yymmdd") &amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>i-VN-AKIRA-231030-01-005</v>
+        <v>i-VN-AKIRA-231101-01-005</v>
       </c>
       <c r="C10" s="29" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>30 Oct 2023</v>
+        <v>01 Nov 2023</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -15011,11 +15014,11 @@
       </c>
       <c r="B11" t="str">
         <f ca="1">"i-VN-AKIRA-"&amp;TEXT(TODAY(),"yymmdd") &amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>i-VN-AKIRA-231030-01-005</v>
+        <v>i-VN-AKIRA-231101-01-005</v>
       </c>
       <c r="C11" s="29" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>30 Oct 2023</v>
+        <v>01 Nov 2023</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -15024,11 +15027,11 @@
       </c>
       <c r="B12" t="str">
         <f ca="1">"i-VN-AKIRA-"&amp;TEXT(TODAY(),"yymmdd") &amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>i-VN-AKIRA-231030-01-005</v>
+        <v>i-VN-AKIRA-231101-01-005</v>
       </c>
       <c r="C12" s="29" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>30 Oct 2023</v>
+        <v>01 Nov 2023</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -15037,11 +15040,11 @@
       </c>
       <c r="B13" t="str">
         <f ca="1">"i-VN-AKIRA-"&amp;TEXT(TODAY(),"yymmdd") &amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>i-VN-AKIRA-231030-01-005</v>
+        <v>i-VN-AKIRA-231101-01-005</v>
       </c>
       <c r="C13" s="29" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>30 Oct 2023</v>
+        <v>01 Nov 2023</v>
       </c>
       <c r="D13" s="43">
         <v>1</v>
@@ -15059,11 +15062,11 @@
       </c>
       <c r="B14" t="str">
         <f ca="1">"i-VN-AKIRA-"&amp;TEXT(TODAY(),"yymmdd") &amp; "-02-0"&amp;AutoIncrement!A2</f>
-        <v>i-VN-AKIRA-231030-02-005</v>
+        <v>i-VN-AKIRA-231101-02-005</v>
       </c>
       <c r="C14" s="29" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>30 Oct 2023</v>
+        <v>01 Nov 2023</v>
       </c>
       <c r="D14" s="43">
         <v>1</v>
@@ -15081,11 +15084,11 @@
       </c>
       <c r="B15" t="str">
         <f ca="1">"i-VN-AKIRA-"&amp;TEXT(TODAY(),"yymmdd") &amp; "-02-0"&amp;AutoIncrement!A2</f>
-        <v>i-VN-AKIRA-231030-02-005</v>
+        <v>i-VN-AKIRA-231101-02-005</v>
       </c>
       <c r="C15" s="29" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>30 Oct 2023</v>
+        <v>01 Nov 2023</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Link TCs SC10 and SC1 to Jira
</commit_message>
<xml_diff>
--- a/Excel Files/Scenario 12/S12_TestCases_Data.xlsx
+++ b/Excel Files/Scenario 12/S12_TestCases_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nasin\git\tb-ttap-brivge-v2\Excel Files\Scenario 12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{784C1B7C-D655-49D2-B07C-BF8E63AA5DFE}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{0B68BC91-1F57-4FB9-8685-7BC487B4293C}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
     <workbookView activeTab="1" tabRatio="621" windowHeight="12456" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
   </bookViews>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1769" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1768" uniqueCount="504">
   <si>
     <t>No</t>
   </si>
@@ -1605,15 +1605,6 @@
     <t>AB</t>
   </si>
   <si>
-    <t>R-VN-TTVN-2311007</t>
-  </si>
-  <si>
-    <t>CR-VN-TTVN-2311006</t>
-  </si>
-  <si>
-    <t>R-SG-TTAP-2311009</t>
-  </si>
-  <si>
     <t>o-SG-BAFCO-231108009</t>
   </si>
   <si>
@@ -1653,9 +1644,6 @@
     <t>TTAP2311018</t>
   </si>
   <si>
-    <t>03</t>
-  </si>
-  <si>
     <t>R-VN-TTVN-2311009</t>
   </si>
   <si>
@@ -1663,6 +1651,18 @@
   </si>
   <si>
     <t>R-SG-TTAP-2311012</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>R-VN-TTVN-2311010</t>
+  </si>
+  <si>
+    <t>CR-VN-TTVN-2311009</t>
+  </si>
+  <si>
+    <t>R-SG-TTAP-2311013</t>
   </si>
 </sst>
 </file>
@@ -3109,7 +3109,7 @@
       </c>
       <c r="B2" s="12" t="str">
         <f>'TC4'!C2</f>
-        <v>SGTTAP-VNTTVN-AB-03-003</v>
+        <v>SGTTAP-VNTTVN-AB-04-004</v>
       </c>
     </row>
   </sheetData>
@@ -3168,7 +3168,7 @@
       </c>
       <c r="D2" s="12" t="str">
         <f>'TC4'!C2</f>
-        <v>SGTTAP-VNTTVN-AB-03-003</v>
+        <v>SGTTAP-VNTTVN-AB-04-004</v>
       </c>
       <c r="E2" s="12" t="str">
         <f>'TC4'!L2</f>
@@ -3192,7 +3192,7 @@
       </c>
       <c r="D3" s="12" t="str">
         <f>'TC4'!C2</f>
-        <v>SGTTAP-VNTTVN-AB-03-003</v>
+        <v>SGTTAP-VNTTVN-AB-04-004</v>
       </c>
       <c r="E3" s="12" t="str">
         <f>'TC4'!L2</f>
@@ -3216,7 +3216,7 @@
       </c>
       <c r="D4" s="12" t="str">
         <f>'TC4'!C2</f>
-        <v>SGTTAP-VNTTVN-AB-03-003</v>
+        <v>SGTTAP-VNTTVN-AB-04-004</v>
       </c>
       <c r="E4" s="12" t="str">
         <f>'TC4'!L2</f>
@@ -3240,7 +3240,7 @@
       </c>
       <c r="D5" s="12" t="str">
         <f>'TC4'!C2</f>
-        <v>SGTTAP-VNTTVN-AB-03-003</v>
+        <v>SGTTAP-VNTTVN-AB-04-004</v>
       </c>
       <c r="E5" s="12" t="str">
         <f>'TC4'!L2</f>
@@ -3264,7 +3264,7 @@
       </c>
       <c r="D6" s="12" t="str">
         <f>'TC4'!C2</f>
-        <v>SGTTAP-VNTTVN-AB-03-003</v>
+        <v>SGTTAP-VNTTVN-AB-04-004</v>
       </c>
       <c r="E6" s="12" t="str">
         <f>'TC4'!L2</f>
@@ -3288,7 +3288,7 @@
       </c>
       <c r="D7" s="12" t="str">
         <f>'TC4'!C2</f>
-        <v>SGTTAP-VNTTVN-AB-03-003</v>
+        <v>SGTTAP-VNTTVN-AB-04-004</v>
       </c>
       <c r="E7" s="12" t="str">
         <f>'TC4'!L2</f>
@@ -3710,7 +3710,7 @@
       </c>
       <c r="D2" s="12" t="str">
         <f>'TC7'!C2</f>
-        <v>SGBAFCO-SGTTAP-ABs-03-003</v>
+        <v>SGBAFCO-SGTTAP-ABs-04-004</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>193</v>
@@ -3738,7 +3738,7 @@
       </c>
       <c r="D3" s="52" t="str">
         <f>'TC7'!C2</f>
-        <v>SGBAFCO-SGTTAP-ABs-03-003</v>
+        <v>SGBAFCO-SGTTAP-ABs-04-004</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>194</v>
@@ -3766,7 +3766,7 @@
       </c>
       <c r="D4" s="52" t="str">
         <f>'TC7'!C2</f>
-        <v>SGBAFCO-SGTTAP-ABs-03-003</v>
+        <v>SGBAFCO-SGTTAP-ABs-04-004</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>195</v>
@@ -3794,7 +3794,7 @@
       </c>
       <c r="D5" s="52" t="str">
         <f>'TC7'!C2</f>
-        <v>SGBAFCO-SGTTAP-ABs-03-003</v>
+        <v>SGBAFCO-SGTTAP-ABs-04-004</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>270</v>
@@ -3822,7 +3822,7 @@
       </c>
       <c r="D6" s="52" t="str">
         <f>'TC7'!C2</f>
-        <v>SGBAFCO-SGTTAP-ABs-03-003</v>
+        <v>SGBAFCO-SGTTAP-ABs-04-004</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>195</v>
@@ -3850,7 +3850,7 @@
       </c>
       <c r="D7" s="52" t="str">
         <f>'TC7'!C2</f>
-        <v>SGBAFCO-SGTTAP-ABs-03-003</v>
+        <v>SGBAFCO-SGTTAP-ABs-04-004</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>195</v>
@@ -3973,7 +3973,7 @@
       </c>
       <c r="C2" s="12" t="str">
         <f>"SGBAFCO-SGTTAP-"&amp;'TC7'!H2&amp;"-0"&amp;AutoIncrement!A2</f>
-        <v>SGBAFCO-SGTTAP-ABs-03-003</v>
+        <v>SGBAFCO-SGTTAP-ABs-04-004</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>37</v>
@@ -3989,11 +3989,11 @@
       </c>
       <c r="H2" s="12" t="str">
         <f>AutoIncrement!C2&amp;"-"&amp;AutoIncrement!A2</f>
-        <v>ABs-03</v>
+        <v>ABs-04</v>
       </c>
       <c r="I2" s="12" t="str">
         <f>"CD-"&amp;H2</f>
-        <v>CD-ABs-03</v>
+        <v>CD-ABs-04</v>
       </c>
       <c r="J2" s="12" t="str">
         <f>'TC6.1'!B2&amp;"("&amp;'TC6.1'!C2&amp;")"</f>
@@ -4027,7 +4027,7 @@
       </c>
       <c r="S2" s="12" t="str">
         <f>'TC4'!N2</f>
-        <v>RD-AB-03</v>
+        <v>RD-AB-04</v>
       </c>
       <c r="T2" t="s">
         <v>502</v>
@@ -4091,7 +4091,7 @@
       </c>
       <c r="D2" s="12" t="str">
         <f>'TC7'!C2</f>
-        <v>SGBAFCO-SGTTAP-ABs-03-003</v>
+        <v>SGBAFCO-SGTTAP-ABs-04-004</v>
       </c>
       <c r="E2" s="24" t="s">
         <v>22</v>
@@ -4117,7 +4117,7 @@
       </c>
       <c r="D3" s="12" t="str">
         <f>'TC7'!C2</f>
-        <v>SGBAFCO-SGTTAP-ABs-03-003</v>
+        <v>SGBAFCO-SGTTAP-ABs-04-004</v>
       </c>
       <c r="E3" s="24" t="s">
         <v>22</v>
@@ -4143,7 +4143,7 @@
       </c>
       <c r="D4" s="12" t="str">
         <f>'TC7'!C2</f>
-        <v>SGBAFCO-SGTTAP-ABs-03-003</v>
+        <v>SGBAFCO-SGTTAP-ABs-04-004</v>
       </c>
       <c r="E4" s="24" t="s">
         <v>22</v>
@@ -4169,7 +4169,7 @@
       </c>
       <c r="D5" s="12" t="str">
         <f>'TC7'!C2</f>
-        <v>SGBAFCO-SGTTAP-ABs-03-003</v>
+        <v>SGBAFCO-SGTTAP-ABs-04-004</v>
       </c>
       <c r="E5" s="24" t="s">
         <v>22</v>
@@ -4195,7 +4195,7 @@
       </c>
       <c r="D6" s="12" t="str">
         <f>'TC7'!C2</f>
-        <v>SGBAFCO-SGTTAP-ABs-03-003</v>
+        <v>SGBAFCO-SGTTAP-ABs-04-004</v>
       </c>
       <c r="E6" s="24" t="s">
         <v>22</v>
@@ -4221,7 +4221,7 @@
       </c>
       <c r="D7" s="12" t="str">
         <f>'TC7'!C2</f>
-        <v>SGBAFCO-SGTTAP-ABs-03-003</v>
+        <v>SGBAFCO-SGTTAP-ABs-04-004</v>
       </c>
       <c r="E7" s="24" t="s">
         <v>22</v>
@@ -4272,7 +4272,7 @@
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="str">
         <f>"CS-"&amp;AutoIncrement!B2&amp;"-"&amp;AutoIncrement!A2</f>
-        <v>CS-AB-03</v>
+        <v>CS-AB-04</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>34</v>
@@ -4282,7 +4282,7 @@
       </c>
       <c r="D2" s="12" t="str">
         <f>'TC4'!C2</f>
-        <v>SGTTAP-VNTTVN-AB-03-003</v>
+        <v>SGTTAP-VNTTVN-AB-04-004</v>
       </c>
     </row>
   </sheetData>
@@ -4321,7 +4321,7 @@
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="str">
         <f>"CS-"&amp;AutoIncrement!C2&amp;"-"&amp;AutoIncrement!A2</f>
-        <v>CS-ABs-03</v>
+        <v>CS-ABs-04</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>34</v>
@@ -4331,7 +4331,7 @@
       </c>
       <c r="D2" s="12" t="str">
         <f>'TC7'!C2</f>
-        <v>SGBAFCO-SGTTAP-ABs-03-003</v>
+        <v>SGBAFCO-SGTTAP-ABs-04-004</v>
       </c>
     </row>
   </sheetData>
@@ -4347,7 +4347,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -4581,11 +4581,11 @@
       </c>
       <c r="B2" s="12" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY())+2, DAY(TODAY())), "dd MMM yyyy")</f>
-        <v>10 Jan 2024</v>
+        <v>13 Jan 2024</v>
       </c>
       <c r="C2" s="12" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY())+3, DAY(TODAY())), "dd MMM yyyy")</f>
-        <v>10 Feb 2024</v>
+        <v>13 Feb 2024</v>
       </c>
     </row>
   </sheetData>
@@ -4718,7 +4718,7 @@
       </c>
       <c r="B2" s="12" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY())+2, DAY(TODAY())+10), "dd MMM yyyy")</f>
-        <v>20 Jan 2024</v>
+        <v>23 Jan 2024</v>
       </c>
     </row>
   </sheetData>
@@ -4758,11 +4758,11 @@
       </c>
       <c r="B2" s="12" t="str">
         <f ca="1">"c" &amp; AutoIncrement!B2&amp;AutoIncrement!A2&amp;"-23"&amp;TEXT(TODAY(),"mm")&amp;"001"</f>
-        <v>cAB03-2311001</v>
+        <v>cAB04-2311001</v>
       </c>
       <c r="C2" s="12" t="str">
         <f ca="1">"c" &amp; AutoIncrement!B2&amp;AutoIncrement!A2&amp;"-23"&amp;TEXT(TODAY(),"mm")&amp;"002"</f>
-        <v>cAB03-2311002</v>
+        <v>cAB04-2311002</v>
       </c>
     </row>
   </sheetData>
@@ -4790,7 +4790,7 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="str">
         <f ca="1">TEXT(TODAY() - WEEKDAY(TODAY(), 2) + 1, "[$-409]mmm d, yyyy") &amp; " ~ " &amp; TEXT(TODAY() - WEEKDAY(TODAY(), 2) + 7, "[$-409]mmm d, yyyy")</f>
-        <v>Nov 6, 2023 ~ Nov 12, 2023</v>
+        <v>Nov 13, 2023 ~ Nov 19, 2023</v>
       </c>
     </row>
   </sheetData>
@@ -4825,7 +4825,7 @@
       </c>
       <c r="B2" s="12" t="str">
         <f>'TC4'!C2</f>
-        <v>SGTTAP-VNTTVN-AB-03-003</v>
+        <v>SGTTAP-VNTTVN-AB-04-004</v>
       </c>
     </row>
   </sheetData>
@@ -4863,11 +4863,11 @@
       </c>
       <c r="B2" s="12" t="str">
         <f ca="1">"s" &amp; AutoIncrement!B2&amp;AutoIncrement!A2&amp;"-23"&amp;TEXT(TODAY(),"mm")&amp;"001"</f>
-        <v>sAB03-2311001</v>
+        <v>sAB04-2311001</v>
       </c>
       <c r="C2" s="12" t="str">
         <f ca="1">"s" &amp; AutoIncrement!B2&amp;AutoIncrement!A2&amp;"-23"&amp;TEXT(TODAY(),"mm")&amp;"002"</f>
-        <v>sAB03-2311002</v>
+        <v>sAB04-2311002</v>
       </c>
     </row>
   </sheetData>
@@ -4905,11 +4905,11 @@
       </c>
       <c r="B2" s="12" t="str">
         <f ca="1">"p" &amp; AutoIncrement!C2&amp;AutoIncrement!A2&amp;"-23"&amp;TEXT(TODAY(),"mm")&amp;"001"</f>
-        <v>pABs03-2311001</v>
+        <v>pABs04-2311001</v>
       </c>
       <c r="C2" s="12" t="str">
         <f ca="1">"p" &amp; AutoIncrement!C2&amp;AutoIncrement!A2&amp;"-23"&amp;TEXT(TODAY(),"mm")&amp;"002"</f>
-        <v>pABs03-2311002</v>
+        <v>pABs04-2311002</v>
       </c>
     </row>
   </sheetData>
@@ -4947,11 +4947,11 @@
       </c>
       <c r="B2" s="12" t="str">
         <f ca="1">"s" &amp; AutoIncrement!C2&amp;AutoIncrement!A2&amp;"-23"&amp;TEXT(TODAY(),"mm")&amp;"001"</f>
-        <v>sABs03-2311001</v>
+        <v>sABs04-2311001</v>
       </c>
       <c r="C2" s="12" t="str">
         <f ca="1">"s" &amp; AutoIncrement!C2&amp;AutoIncrement!A2&amp;"-23"&amp;TEXT(TODAY(),"mm")&amp;"002"</f>
-        <v>sABs03-2311002</v>
+        <v>sABs04-2311002</v>
       </c>
     </row>
   </sheetData>
@@ -5517,7 +5517,7 @@
       </c>
       <c r="D2" s="22" t="str">
         <f ca="1">"rc"&amp;AutoIncrement!B2&amp;AutoIncrement!A2&amp;"-23"&amp;TEXT(TODAY(),"mm")&amp;"001-01"</f>
-        <v>rcAB03-2311001-01</v>
+        <v>rcAB04-2311001-01</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -6021,7 +6021,7 @@
       </c>
       <c r="D2" s="22" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sAB03-2311001</v>
+        <v>sAB04-2311001</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>81</v>
@@ -6051,7 +6051,7 @@
       </c>
       <c r="D3" s="22" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sAB03-2311001</v>
+        <v>sAB04-2311001</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>81</v>
@@ -6081,7 +6081,7 @@
       </c>
       <c r="D4" s="22" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sAB03-2311001</v>
+        <v>sAB04-2311001</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>81</v>
@@ -6111,7 +6111,7 @@
       </c>
       <c r="D5" s="22" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sAB03-2311001</v>
+        <v>sAB04-2311001</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>81</v>
@@ -6141,7 +6141,7 @@
       </c>
       <c r="D6" s="22" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sAB03-2311001</v>
+        <v>sAB04-2311001</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>81</v>
@@ -6171,7 +6171,7 @@
       </c>
       <c r="D7" s="22" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sAB03-2311001</v>
+        <v>sAB04-2311001</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>81</v>
@@ -6249,7 +6249,7 @@
       </c>
       <c r="D2" s="22" t="str">
         <f ca="1">'TC11-Customer CO'!B2</f>
-        <v>cAB03-2311001</v>
+        <v>cAB04-2311001</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>34</v>
@@ -6279,7 +6279,7 @@
       </c>
       <c r="D3" s="22" t="str">
         <f ca="1">'TC11-Customer CO'!B2</f>
-        <v>cAB03-2311001</v>
+        <v>cAB04-2311001</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>34</v>
@@ -6309,7 +6309,7 @@
       </c>
       <c r="D4" s="22" t="str">
         <f ca="1">'TC11-Customer CO'!B2</f>
-        <v>cAB03-2311001</v>
+        <v>cAB04-2311001</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>34</v>
@@ -6339,7 +6339,7 @@
       </c>
       <c r="D5" s="22" t="str">
         <f ca="1">'TC11-Customer CO'!B2</f>
-        <v>cAB03-2311001</v>
+        <v>cAB04-2311001</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>34</v>
@@ -6369,7 +6369,7 @@
       </c>
       <c r="D6" s="22" t="str">
         <f ca="1">'TC11-Customer CO'!B2</f>
-        <v>cAB03-2311001</v>
+        <v>cAB04-2311001</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>34</v>
@@ -6399,7 +6399,7 @@
       </c>
       <c r="D7" s="22" t="str">
         <f ca="1">'TC11-Customer CO'!B2</f>
-        <v>cAB03-2311001</v>
+        <v>cAB04-2311001</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>34</v>
@@ -6684,7 +6684,7 @@
       <c r="C2" s="22"/>
       <c r="D2" s="22" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sAB03-2311001</v>
+        <v>sAB04-2311001</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>81</v>
@@ -6712,7 +6712,7 @@
       <c r="C3" s="22"/>
       <c r="D3" s="22" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sAB03-2311001</v>
+        <v>sAB04-2311001</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>81</v>
@@ -6740,7 +6740,7 @@
       <c r="C4" s="22"/>
       <c r="D4" s="22" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sAB03-2311001</v>
+        <v>sAB04-2311001</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>81</v>
@@ -6768,7 +6768,7 @@
       <c r="C5" s="22"/>
       <c r="D5" s="22" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sAB03-2311001</v>
+        <v>sAB04-2311001</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>81</v>
@@ -6796,7 +6796,7 @@
       <c r="C6" s="22"/>
       <c r="D6" s="22" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sAB03-2311001</v>
+        <v>sAB04-2311001</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>81</v>
@@ -6824,7 +6824,7 @@
       <c r="C7" s="22"/>
       <c r="D7" s="22" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sAB03-2311001</v>
+        <v>sAB04-2311001</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>81</v>
@@ -7029,15 +7029,15 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY())+2, DAY(TODAY())), "dd MMM yyyy")</f>
-        <v>10 Jan 2024</v>
+        <v>13 Jan 2024</v>
       </c>
       <c r="B2" s="12" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY())+3, DAY(TODAY())), "dd MMM yyyy")</f>
-        <v>10 Feb 2024</v>
+        <v>13 Feb 2024</v>
       </c>
       <c r="C2" s="12" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY())+4, DAY(TODAY())), "dd MMM yyyy")</f>
-        <v>10 Mar 2024</v>
+        <v>13 Mar 2024</v>
       </c>
     </row>
   </sheetData>
@@ -7065,7 +7065,7 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="str">
         <f ca="1">"rc"&amp;AutoIncrement!B2&amp;AutoIncrement!A2&amp;"-23"&amp;TEXT(TODAY(),"mm")&amp;"001-02"</f>
-        <v>rcAB03-2311001-02</v>
+        <v>rcAB04-2311001-02</v>
       </c>
     </row>
   </sheetData>
@@ -8180,7 +8180,7 @@
       </c>
       <c r="D2" s="12" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sAB03-2311001</v>
+        <v>sAB04-2311001</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>81</v>
@@ -8244,7 +8244,7 @@
       </c>
       <c r="D3" s="12" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sAB03-2311001</v>
+        <v>sAB04-2311001</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>81</v>
@@ -8307,7 +8307,7 @@
       </c>
       <c r="D4" s="12" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sAB03-2311001</v>
+        <v>sAB04-2311001</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>81</v>
@@ -8370,7 +8370,7 @@
       </c>
       <c r="D5" s="12" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sAB03-2311001</v>
+        <v>sAB04-2311001</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>81</v>
@@ -8433,7 +8433,7 @@
       </c>
       <c r="D6" s="12" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sAB03-2311001</v>
+        <v>sAB04-2311001</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>81</v>
@@ -8495,7 +8495,7 @@
       </c>
       <c r="D7" s="12" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sAB03-2311001</v>
+        <v>sAB04-2311001</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>81</v>
@@ -8652,7 +8652,7 @@
       </c>
       <c r="D2" s="12" t="str">
         <f ca="1">'TC11-Customer CO'!B2</f>
-        <v>cAB03-2311001</v>
+        <v>cAB04-2311001</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>34</v>
@@ -8728,7 +8728,7 @@
       </c>
       <c r="D3" s="12" t="str">
         <f ca="1">'TC11-Customer CO'!B2</f>
-        <v>cAB03-2311001</v>
+        <v>cAB04-2311001</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>34</v>
@@ -8804,7 +8804,7 @@
       </c>
       <c r="D4" s="12" t="str">
         <f ca="1">'TC11-Customer CO'!B2</f>
-        <v>cAB03-2311001</v>
+        <v>cAB04-2311001</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>34</v>
@@ -8880,7 +8880,7 @@
       </c>
       <c r="D5" s="12" t="str">
         <f ca="1">'TC11-Customer CO'!B2</f>
-        <v>cAB03-2311001</v>
+        <v>cAB04-2311001</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>34</v>
@@ -8956,7 +8956,7 @@
       </c>
       <c r="D6" s="12" t="str">
         <f ca="1">'TC11-Customer CO'!B2</f>
-        <v>cAB03-2311001</v>
+        <v>cAB04-2311001</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>34</v>
@@ -9032,7 +9032,7 @@
       </c>
       <c r="D7" s="12" t="str">
         <f ca="1">'TC11-Customer CO'!B2</f>
-        <v>cAB03-2311001</v>
+        <v>cAB04-2311001</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>34</v>
@@ -9186,7 +9186,7 @@
       <c r="C2" s="22"/>
       <c r="D2" s="12" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sAB03-2311001</v>
+        <v>sAB04-2311001</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>81</v>
@@ -9245,7 +9245,7 @@
       <c r="C3" s="22"/>
       <c r="D3" s="12" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sAB03-2311001</v>
+        <v>sAB04-2311001</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>81</v>
@@ -9304,7 +9304,7 @@
       <c r="C4" s="22"/>
       <c r="D4" s="12" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sAB03-2311001</v>
+        <v>sAB04-2311001</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>81</v>
@@ -9363,7 +9363,7 @@
       <c r="C5" s="22"/>
       <c r="D5" s="12" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sAB03-2311001</v>
+        <v>sAB04-2311001</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>81</v>
@@ -9422,7 +9422,7 @@
       <c r="C6" s="22"/>
       <c r="D6" s="12" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sAB03-2311001</v>
+        <v>sAB04-2311001</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>81</v>
@@ -9481,7 +9481,7 @@
       <c r="C7" s="22"/>
       <c r="D7" s="12" t="str">
         <f ca="1">'TC14-BU SO'!B2</f>
-        <v>sAB03-2311001</v>
+        <v>sAB04-2311001</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>81</v>
@@ -9565,7 +9565,7 @@
       </c>
       <c r="B2" s="22" t="str">
         <f>"RequestPart-"&amp;'TC4'!H2</f>
-        <v>RequestPart-AB-03</v>
+        <v>RequestPart-AB-04</v>
       </c>
       <c r="C2" s="5"/>
     </row>
@@ -9673,7 +9673,7 @@
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="str">
         <f ca="1">'TC15-BU PO'!B2</f>
-        <v>pABs03-2311001</v>
+        <v>pABs04-2311001</v>
       </c>
       <c r="E2" s="22" t="s">
         <v>34</v>
@@ -9747,7 +9747,7 @@
       <c r="C3" s="12"/>
       <c r="D3" s="12" t="str">
         <f ca="1">'TC15-BU PO'!B2</f>
-        <v>pABs03-2311001</v>
+        <v>pABs04-2311001</v>
       </c>
       <c r="E3" s="22" t="s">
         <v>34</v>
@@ -9821,7 +9821,7 @@
       <c r="C4" s="12"/>
       <c r="D4" s="12" t="str">
         <f ca="1">'TC15-BU PO'!B2</f>
-        <v>pABs03-2311001</v>
+        <v>pABs04-2311001</v>
       </c>
       <c r="E4" s="22" t="s">
         <v>34</v>
@@ -9895,7 +9895,7 @@
       <c r="C5" s="12"/>
       <c r="D5" s="12" t="str">
         <f ca="1">'TC15-BU PO'!B2</f>
-        <v>pABs03-2311001</v>
+        <v>pABs04-2311001</v>
       </c>
       <c r="E5" s="22" t="s">
         <v>34</v>
@@ -9969,7 +9969,7 @@
       <c r="C6" s="12"/>
       <c r="D6" s="12" t="str">
         <f ca="1">'TC15-BU PO'!B2</f>
-        <v>pABs03-2311001</v>
+        <v>pABs04-2311001</v>
       </c>
       <c r="E6" s="22" t="s">
         <v>34</v>
@@ -10043,7 +10043,7 @@
       <c r="C7" s="12"/>
       <c r="D7" s="12" t="str">
         <f ca="1">'TC15-BU PO'!B2</f>
-        <v>pABs03-2311001</v>
+        <v>pABs04-2311001</v>
       </c>
       <c r="E7" s="22" t="s">
         <v>34</v>
@@ -10148,19 +10148,19 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY())+1, DAY(TODAY())), "dd MMM yyyy")</f>
-        <v>10 Dec 2023</v>
+        <v>13 Dec 2023</v>
       </c>
       <c r="B2" s="12" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY())+2, DAY(TODAY())), "dd MMM yyyy")</f>
-        <v>10 Jan 2024</v>
+        <v>13 Jan 2024</v>
       </c>
       <c r="C2" s="12" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY())+3, DAY(TODAY())), "dd MMM yyyy")</f>
-        <v>10 Feb 2024</v>
+        <v>13 Feb 2024</v>
       </c>
       <c r="D2" s="12" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY())+4, DAY(TODAY())), "dd MMM yyyy")</f>
-        <v>10 Mar 2024</v>
+        <v>13 Mar 2024</v>
       </c>
       <c r="E2" s="12"/>
     </row>
@@ -10357,7 +10357,7 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="str">
         <f ca="1">"rs"&amp;AutoIncrement!C2&amp;AutoIncrement!A2&amp;"-23"&amp;TEXT(TODAY(),"mm")&amp;"001-01"</f>
-        <v>rsABs03-2311001-01</v>
+        <v>rsABs04-2311001-01</v>
       </c>
     </row>
   </sheetData>
@@ -11910,26 +11910,26 @@
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="36" t="str">
         <f ca="1"><![CDATA["o-SG-BAFCO-"&TEXT(TODAY(),"yymm")&"-"&AutoIncrement!B2&"-"&AutoIncrement!A2&"-001"]]></f>
-        <v>o-SG-BAFCO-2311-AB-03-001</v>
+        <v>o-SG-BAFCO-2311-AB-04-001</v>
       </c>
       <c r="B3" s="37" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY()), DAY(TODAY())-1), "dd MMM yyyy")</f>
-        <v>09 Nov 2023</v>
+        <v>12 Nov 2023</v>
       </c>
       <c r="C3" s="37" t="str">
         <f ca="1">"B-"&amp;TEXT(TODAY(),"yymm")&amp;"-"&amp;AutoIncrement!B2&amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>B-2311-AB-01-003</v>
+        <v>B-2311-AB-01-004</v>
       </c>
       <c r="D3" s="38">
         <v>1000</v>
       </c>
       <c r="E3" s="37" t="str">
         <f ca="1" ref="E3:E8" si="0" t="shared">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY()), DAY(TODAY())+2), "dd MMM yyyy")</f>
-        <v>12 Nov 2023</v>
+        <v>15 Nov 2023</v>
       </c>
       <c r="F3" s="37" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY()), DAY(TODAY())+10), "dd MMM yyyy")</f>
-        <v>20 Nov 2023</v>
+        <v>23 Nov 2023</v>
       </c>
       <c r="G3" s="39"/>
       <c r="H3" s="28"/>
@@ -11940,7 +11940,7 @@
       <c r="M3" s="40"/>
       <c r="N3" s="37" t="str">
         <f ca="1">"OP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>OP-231110-01-003</v>
+        <v>OP-231113-01-004</v>
       </c>
       <c r="O3" s="28" t="s">
         <v>222</v>
@@ -11956,7 +11956,7 @@
       </c>
       <c r="S3" s="37" t="str">
         <f ca="1">"IP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>IP-231110-01-003</v>
+        <v>IP-231113-01-004</v>
       </c>
       <c r="T3" s="42"/>
       <c r="U3" s="41">
@@ -11972,26 +11972,26 @@
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="36" t="str">
         <f ca="1"><![CDATA["o-SG-BAFCO-"&TEXT(TODAY(),"yymm")&"-"&AutoIncrement!B2&"-"&AutoIncrement!A2&"-001"]]></f>
-        <v>o-SG-BAFCO-2311-AB-03-001</v>
+        <v>o-SG-BAFCO-2311-AB-04-001</v>
       </c>
       <c r="B4" s="37" t="str">
         <f ca="1" ref="B4:B8" si="1" t="shared">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY()), DAY(TODAY())-1), "dd MMM yyyy")</f>
-        <v>09 Nov 2023</v>
+        <v>12 Nov 2023</v>
       </c>
       <c r="C4" s="37" t="str">
         <f ca="1">"B-"&amp;TEXT(TODAY(),"yymm")&amp;"-"&amp;AutoIncrement!B2&amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>B-2311-AB-01-003</v>
+        <v>B-2311-AB-01-004</v>
       </c>
       <c r="D4" s="38">
         <v>800</v>
       </c>
       <c r="E4" s="37" t="str">
         <f ca="1" si="0" t="shared"/>
-        <v>12 Nov 2023</v>
+        <v>15 Nov 2023</v>
       </c>
       <c r="F4" s="37" t="str">
         <f ca="1" ref="F4:F8" si="2" t="shared">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY()), DAY(TODAY())+10), "dd MMM yyyy")</f>
-        <v>20 Nov 2023</v>
+        <v>23 Nov 2023</v>
       </c>
       <c r="G4" s="39" t="s">
         <v>240</v>
@@ -12004,7 +12004,7 @@
       <c r="M4" s="40"/>
       <c r="N4" s="37" t="str">
         <f ca="1">"OP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>OP-231110-01-003</v>
+        <v>OP-231113-01-004</v>
       </c>
       <c r="O4" s="28" t="s">
         <v>223</v>
@@ -12020,7 +12020,7 @@
       </c>
       <c r="S4" s="37" t="str">
         <f ca="1">"IP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-02-0"&amp;AutoIncrement!A2</f>
-        <v>IP-231110-02-003</v>
+        <v>IP-231113-02-004</v>
       </c>
       <c r="T4" s="42" t="s">
         <v>232</v>
@@ -12038,26 +12038,26 @@
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="36" t="str">
         <f ca="1"><![CDATA["o-SG-BAFCO-"&TEXT(TODAY(),"yymm")&"-"&AutoIncrement!B2&"-"&AutoIncrement!A2&"-001"]]></f>
-        <v>o-SG-BAFCO-2311-AB-03-001</v>
+        <v>o-SG-BAFCO-2311-AB-04-001</v>
       </c>
       <c r="B5" s="37" t="str">
         <f ca="1" si="1" t="shared"/>
-        <v>09 Nov 2023</v>
+        <v>12 Nov 2023</v>
       </c>
       <c r="C5" s="37" t="str">
         <f ca="1">"B-"&amp;TEXT(TODAY(),"yymm")&amp;"-"&amp;AutoIncrement!B2&amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>B-2311-AB-01-003</v>
+        <v>B-2311-AB-01-004</v>
       </c>
       <c r="D5" s="38">
         <v>900</v>
       </c>
       <c r="E5" s="37" t="str">
         <f ca="1" si="0" t="shared"/>
-        <v>12 Nov 2023</v>
+        <v>15 Nov 2023</v>
       </c>
       <c r="F5" s="37" t="str">
         <f ca="1" si="2" t="shared"/>
-        <v>20 Nov 2023</v>
+        <v>23 Nov 2023</v>
       </c>
       <c r="G5" s="39" t="s">
         <v>220</v>
@@ -12080,7 +12080,7 @@
       </c>
       <c r="N5" s="37" t="str">
         <f ca="1">"OP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-02-0"&amp;AutoIncrement!A2</f>
-        <v>OP-231110-02-003</v>
+        <v>OP-231113-02-004</v>
       </c>
       <c r="O5" s="28" t="s">
         <v>223</v>
@@ -12103,26 +12103,26 @@
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="36" t="str">
         <f ca="1"><![CDATA["o-SG-BAFCO-"&TEXT(TODAY(),"yymm")&"-"&AutoIncrement!B2&"-"&AutoIncrement!A2&"-001"]]></f>
-        <v>o-SG-BAFCO-2311-AB-03-001</v>
+        <v>o-SG-BAFCO-2311-AB-04-001</v>
       </c>
       <c r="B6" s="37" t="str">
         <f ca="1" si="1" t="shared"/>
-        <v>09 Nov 2023</v>
+        <v>12 Nov 2023</v>
       </c>
       <c r="C6" s="37" t="str">
         <f ca="1">"B-"&amp;TEXT(TODAY(),"yymm")&amp;"-"&amp;AutoIncrement!B2&amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>B-2311-AB-01-003</v>
+        <v>B-2311-AB-01-004</v>
       </c>
       <c r="D6" s="38">
         <v>1200</v>
       </c>
       <c r="E6" s="37" t="str">
         <f ca="1" si="0" t="shared"/>
-        <v>12 Nov 2023</v>
+        <v>15 Nov 2023</v>
       </c>
       <c r="F6" s="37" t="str">
         <f ca="1" si="2" t="shared"/>
-        <v>20 Nov 2023</v>
+        <v>23 Nov 2023</v>
       </c>
       <c r="G6" s="39" t="s">
         <v>220</v>
@@ -12147,7 +12147,7 @@
       </c>
       <c r="N6" s="37" t="str">
         <f ca="1">"OP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-02-0"&amp;AutoIncrement!A2</f>
-        <v>OP-231110-02-003</v>
+        <v>OP-231113-02-004</v>
       </c>
       <c r="O6" s="28" t="s">
         <v>223</v>
@@ -12170,26 +12170,26 @@
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="36" t="str">
         <f ca="1"><![CDATA["o-SG-BAFCO-"&TEXT(TODAY(),"yymm")&"-"&AutoIncrement!B2&"-"&AutoIncrement!A2&"-001"]]></f>
-        <v>o-SG-BAFCO-2311-AB-03-001</v>
+        <v>o-SG-BAFCO-2311-AB-04-001</v>
       </c>
       <c r="B7" s="37" t="str">
         <f ca="1" si="1" t="shared"/>
-        <v>09 Nov 2023</v>
+        <v>12 Nov 2023</v>
       </c>
       <c r="C7" s="37" t="str">
         <f ca="1">"B-"&amp;TEXT(TODAY(),"yymm")&amp;"-"&amp;AutoIncrement!B2&amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>B-2311-AB-01-003</v>
+        <v>B-2311-AB-01-004</v>
       </c>
       <c r="D7" s="38">
         <v>1000</v>
       </c>
       <c r="E7" s="37" t="str">
         <f ca="1" si="0" t="shared"/>
-        <v>12 Nov 2023</v>
+        <v>15 Nov 2023</v>
       </c>
       <c r="F7" s="37" t="str">
         <f ca="1" si="2" t="shared"/>
-        <v>20 Nov 2023</v>
+        <v>23 Nov 2023</v>
       </c>
       <c r="G7" s="39" t="s">
         <v>221</v>
@@ -12214,7 +12214,7 @@
       </c>
       <c r="N7" s="37" t="str">
         <f ca="1">"OP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-03-0"&amp;AutoIncrement!A2</f>
-        <v>OP-231110-03-003</v>
+        <v>OP-231113-03-004</v>
       </c>
       <c r="O7" s="28" t="s">
         <v>224</v>
@@ -12230,7 +12230,7 @@
       </c>
       <c r="S7" s="37" t="str">
         <f ca="1">"IP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>IP-231110-01-003</v>
+        <v>IP-231113-01-004</v>
       </c>
       <c r="T7" s="42" t="s">
         <v>232</v>
@@ -12248,26 +12248,26 @@
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="36" t="str">
         <f ca="1"><![CDATA["o-SG-BAFCO-"&TEXT(TODAY(),"yymm")&"-"&AutoIncrement!B2&"-"&AutoIncrement!A2&"-001"]]></f>
-        <v>o-SG-BAFCO-2311-AB-03-001</v>
+        <v>o-SG-BAFCO-2311-AB-04-001</v>
       </c>
       <c r="B8" s="37" t="str">
         <f ca="1" si="1" t="shared"/>
-        <v>09 Nov 2023</v>
+        <v>12 Nov 2023</v>
       </c>
       <c r="C8" s="37" t="str">
         <f ca="1">"B-"&amp;TEXT(TODAY(),"yymm")&amp;"-"&amp;AutoIncrement!B2&amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>B-2311-AB-01-003</v>
+        <v>B-2311-AB-01-004</v>
       </c>
       <c r="D8" s="38">
         <v>1100</v>
       </c>
       <c r="E8" s="37" t="str">
         <f ca="1" si="0" t="shared"/>
-        <v>12 Nov 2023</v>
+        <v>15 Nov 2023</v>
       </c>
       <c r="F8" s="37" t="str">
         <f ca="1" si="2" t="shared"/>
-        <v>20 Nov 2023</v>
+        <v>23 Nov 2023</v>
       </c>
       <c r="G8" s="39" t="s">
         <v>221</v>
@@ -12292,7 +12292,7 @@
       </c>
       <c r="N8" s="37" t="str">
         <f ca="1">"OP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-03-0"&amp;AutoIncrement!A2</f>
-        <v>OP-231110-03-003</v>
+        <v>OP-231113-03-004</v>
       </c>
       <c r="O8" s="28" t="s">
         <v>224</v>
@@ -12308,7 +12308,7 @@
       </c>
       <c r="S8" s="37" t="str">
         <f ca="1">"IP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-02-0"&amp;AutoIncrement!A2</f>
-        <v>IP-231110-02-003</v>
+        <v>IP-231113-02-004</v>
       </c>
       <c r="T8" s="42" t="s">
         <v>239</v>
@@ -12477,11 +12477,11 @@
       </c>
       <c r="C2" s="36" t="str">
         <f ca="1"><![CDATA["o-SG-BAFCO-"&TEXT(TODAY(),"yymm")&"-"&AutoIncrement!B2&"-"&AutoIncrement!A2&"-002"]]></f>
-        <v>o-SG-BAFCO-2311-AB-03-002</v>
+        <v>o-SG-BAFCO-2311-AB-04-002</v>
       </c>
       <c r="D2" s="37" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY()), DAY(TODAY())-1), "dd MMM yyyy")</f>
-        <v>09 Nov 2023</v>
+        <v>12 Nov 2023</v>
       </c>
       <c r="E2" s="37"/>
       <c r="F2" s="21" t="s">
@@ -12507,11 +12507,11 @@
       </c>
       <c r="M2" s="37" t="str">
         <f ca="1" ref="M2:M9" si="0" t="shared">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY()), DAY(TODAY())+2), "dd MMM yyyy")</f>
-        <v>12 Nov 2023</v>
+        <v>15 Nov 2023</v>
       </c>
       <c r="N2" s="37" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY()), DAY(TODAY())+10), "dd MMM yyyy")</f>
-        <v>20 Nov 2023</v>
+        <v>23 Nov 2023</v>
       </c>
       <c r="O2" s="19" t="s">
         <v>252</v>
@@ -12524,7 +12524,7 @@
       <c r="U2" s="44"/>
       <c r="V2" s="37" t="str">
         <f ca="1">"OP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-02-0"&amp;AutoIncrement!A2</f>
-        <v>OP-231110-02-003</v>
+        <v>OP-231113-02-004</v>
       </c>
       <c r="W2" s="19" t="s">
         <v>253</v>
@@ -12534,7 +12534,7 @@
       <c r="Z2" s="44"/>
       <c r="AA2" s="37" t="str">
         <f ca="1">"IP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>IP-231110-01-003</v>
+        <v>IP-231113-01-004</v>
       </c>
       <c r="AB2" s="45" t="s">
         <v>254</v>
@@ -12544,7 +12544,7 @@
       <c r="AE2" s="44"/>
       <c r="AF2" s="37" t="str">
         <f ca="1">'TC16-Supplier SO'!C2</f>
-        <v>sABs03-2311002</v>
+        <v>sABs04-2311002</v>
       </c>
       <c r="AG2" s="37" t="s">
         <v>81</v>
@@ -12575,11 +12575,11 @@
       </c>
       <c r="C3" s="36" t="str">
         <f ca="1"><![CDATA["o-SG-BAFCO-"&TEXT(TODAY(),"yymm")&"-"&AutoIncrement!B2&"-"&AutoIncrement!A2&"-002"]]></f>
-        <v>o-SG-BAFCO-2311-AB-03-002</v>
+        <v>o-SG-BAFCO-2311-AB-04-002</v>
       </c>
       <c r="D3" s="37" t="str">
         <f ca="1" ref="D3:D9" si="1" t="shared">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY()), DAY(TODAY())-1), "dd MMM yyyy")</f>
-        <v>09 Nov 2023</v>
+        <v>12 Nov 2023</v>
       </c>
       <c r="E3" s="37"/>
       <c r="F3" s="21" t="s">
@@ -12605,11 +12605,11 @@
       </c>
       <c r="M3" s="37" t="str">
         <f ca="1" si="0" t="shared"/>
-        <v>12 Nov 2023</v>
+        <v>15 Nov 2023</v>
       </c>
       <c r="N3" s="37" t="str">
         <f ca="1" ref="N3:N9" si="2" t="shared">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY()), DAY(TODAY())+10), "dd MMM yyyy")</f>
-        <v>20 Nov 2023</v>
+        <v>23 Nov 2023</v>
       </c>
       <c r="O3" s="19" t="s">
         <v>252</v>
@@ -12622,7 +12622,7 @@
       <c r="U3" s="44"/>
       <c r="V3" s="37" t="str">
         <f ca="1">"OP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-02-0"&amp;AutoIncrement!A2</f>
-        <v>OP-231110-02-003</v>
+        <v>OP-231113-02-004</v>
       </c>
       <c r="W3" s="19" t="s">
         <v>253</v>
@@ -12632,7 +12632,7 @@
       <c r="Z3" s="44"/>
       <c r="AA3" s="37" t="str">
         <f ca="1">"IP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-02-0"&amp;AutoIncrement!A2</f>
-        <v>IP-231110-02-003</v>
+        <v>IP-231113-02-004</v>
       </c>
       <c r="AB3" s="45" t="s">
         <v>255</v>
@@ -12642,7 +12642,7 @@
       <c r="AE3" s="44"/>
       <c r="AF3" s="37" t="str">
         <f ca="1">'TC16-Supplier SO'!C2</f>
-        <v>sABs03-2311002</v>
+        <v>sABs04-2311002</v>
       </c>
       <c r="AG3" s="37" t="s">
         <v>81</v>
@@ -12673,11 +12673,11 @@
       </c>
       <c r="C4" s="36" t="str">
         <f ca="1"><![CDATA["o-SG-BAFCO-"&TEXT(TODAY(),"yymm")&"-"&AutoIncrement!B2&"-"&AutoIncrement!A2&"-002"]]></f>
-        <v>o-SG-BAFCO-2311-AB-03-002</v>
+        <v>o-SG-BAFCO-2311-AB-04-002</v>
       </c>
       <c r="D4" s="37" t="str">
         <f ca="1" si="1" t="shared"/>
-        <v>09 Nov 2023</v>
+        <v>12 Nov 2023</v>
       </c>
       <c r="E4" s="37"/>
       <c r="F4" s="21" t="s">
@@ -12703,11 +12703,11 @@
       </c>
       <c r="M4" s="37" t="str">
         <f ca="1" si="0" t="shared"/>
-        <v>12 Nov 2023</v>
+        <v>15 Nov 2023</v>
       </c>
       <c r="N4" s="37" t="str">
         <f ca="1" si="2" t="shared"/>
-        <v>20 Nov 2023</v>
+        <v>23 Nov 2023</v>
       </c>
       <c r="O4" s="39" t="s">
         <v>252</v>
@@ -12720,7 +12720,7 @@
       <c r="U4" s="40"/>
       <c r="V4" s="37" t="str">
         <f ca="1">"OP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>OP-231110-01-003</v>
+        <v>OP-231113-01-004</v>
       </c>
       <c r="W4" s="28" t="s">
         <v>256</v>
@@ -12736,7 +12736,7 @@
       </c>
       <c r="AA4" s="37" t="str">
         <f ca="1">"IP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-02-0"&amp;AutoIncrement!A2</f>
-        <v>IP-231110-02-003</v>
+        <v>IP-231113-02-004</v>
       </c>
       <c r="AB4" s="42" t="s">
         <v>257</v>
@@ -12746,7 +12746,7 @@
       <c r="AE4" s="40"/>
       <c r="AF4" s="37" t="str">
         <f ca="1">'TC16-Supplier SO'!C2</f>
-        <v>sABs03-2311002</v>
+        <v>sABs04-2311002</v>
       </c>
       <c r="AG4" s="37" t="s">
         <v>81</v>
@@ -12777,11 +12777,11 @@
       </c>
       <c r="C5" s="36" t="str">
         <f ca="1"><![CDATA["o-SG-BAFCO-"&TEXT(TODAY(),"yymm")&"-"&AutoIncrement!B2&"-"&AutoIncrement!A2&"-002"]]></f>
-        <v>o-SG-BAFCO-2311-AB-03-002</v>
+        <v>o-SG-BAFCO-2311-AB-04-002</v>
       </c>
       <c r="D5" s="37" t="str">
         <f ca="1" si="1" t="shared"/>
-        <v>09 Nov 2023</v>
+        <v>12 Nov 2023</v>
       </c>
       <c r="E5" s="37"/>
       <c r="F5" s="21" t="s">
@@ -12807,11 +12807,11 @@
       </c>
       <c r="M5" s="37" t="str">
         <f ca="1" si="0" t="shared"/>
-        <v>12 Nov 2023</v>
+        <v>15 Nov 2023</v>
       </c>
       <c r="N5" s="37" t="str">
         <f ca="1" si="2" t="shared"/>
-        <v>20 Nov 2023</v>
+        <v>23 Nov 2023</v>
       </c>
       <c r="O5" s="21" t="s">
         <v>258</v>
@@ -12836,7 +12836,7 @@
       </c>
       <c r="V5" s="37" t="str">
         <f ca="1">"OP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>OP-231110-01-003</v>
+        <v>OP-231113-01-004</v>
       </c>
       <c r="W5" s="19" t="s">
         <v>262</v>
@@ -12846,7 +12846,7 @@
       <c r="Z5" s="44"/>
       <c r="AA5" s="37" t="str">
         <f ca="1">"IP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>IP-231110-01-003</v>
+        <v>IP-231113-01-004</v>
       </c>
       <c r="AB5" s="45"/>
       <c r="AC5" s="44"/>
@@ -12854,7 +12854,7 @@
       <c r="AE5" s="44"/>
       <c r="AF5" s="37" t="str">
         <f ca="1">'TC16-Supplier SO'!C2</f>
-        <v>sABs03-2311002</v>
+        <v>sABs04-2311002</v>
       </c>
       <c r="AG5" s="37" t="s">
         <v>81</v>
@@ -12885,15 +12885,15 @@
       </c>
       <c r="C6" s="36" t="str">
         <f ca="1"><![CDATA["o-SG-BAFCO-"&TEXT(TODAY(),"yymm")&"-"&AutoIncrement!B2&"-"&AutoIncrement!A2&"-003"]]></f>
-        <v>o-SG-BAFCO-2311-AB-03-003</v>
+        <v>o-SG-BAFCO-2311-AB-04-003</v>
       </c>
       <c r="D6" s="37" t="str">
         <f ca="1" si="1" t="shared"/>
-        <v>09 Nov 2023</v>
+        <v>12 Nov 2023</v>
       </c>
       <c r="E6" s="37" t="str">
         <f ca="1">"B-"&amp;TEXT(TODAY(),"yymm")&amp;"-"&amp;AutoIncrement!B2&amp; "-02-0"&amp;AutoIncrement!A2</f>
-        <v>B-2311-AB-02-003</v>
+        <v>B-2311-AB-02-004</v>
       </c>
       <c r="F6" s="21" t="s">
         <v>29</v>
@@ -12918,11 +12918,11 @@
       </c>
       <c r="M6" s="37" t="str">
         <f ca="1" si="0" t="shared"/>
-        <v>12 Nov 2023</v>
+        <v>15 Nov 2023</v>
       </c>
       <c r="N6" s="37" t="str">
         <f ca="1" si="2" t="shared"/>
-        <v>20 Nov 2023</v>
+        <v>23 Nov 2023</v>
       </c>
       <c r="O6" s="21" t="s">
         <v>263</v>
@@ -12939,7 +12939,7 @@
       <c r="U6" s="44"/>
       <c r="V6" s="37" t="str">
         <f ca="1">"OP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>OP-231110-01-003</v>
+        <v>OP-231113-01-004</v>
       </c>
       <c r="W6" s="19" t="s">
         <v>262</v>
@@ -12954,7 +12954,7 @@
       <c r="AE6" s="44"/>
       <c r="AF6" s="37" t="str">
         <f ca="1">'TC16-Supplier SO'!C2</f>
-        <v>sABs03-2311002</v>
+        <v>sABs04-2311002</v>
       </c>
       <c r="AG6" s="37" t="s">
         <v>81</v>
@@ -12985,15 +12985,15 @@
       </c>
       <c r="C7" s="36" t="str">
         <f ca="1"><![CDATA["o-SG-BAFCO-"&TEXT(TODAY(),"yymm")&"-"&AutoIncrement!B2&"-"&AutoIncrement!A2&"-003"]]></f>
-        <v>o-SG-BAFCO-2311-AB-03-003</v>
+        <v>o-SG-BAFCO-2311-AB-04-003</v>
       </c>
       <c r="D7" s="37" t="str">
         <f ca="1" si="1" t="shared"/>
-        <v>09 Nov 2023</v>
+        <v>12 Nov 2023</v>
       </c>
       <c r="E7" s="37" t="str">
         <f ca="1">"B-"&amp;TEXT(TODAY(),"yymm")&amp;"-"&amp;AutoIncrement!B2&amp; "-02-0"&amp;AutoIncrement!A2</f>
-        <v>B-2311-AB-02-003</v>
+        <v>B-2311-AB-02-004</v>
       </c>
       <c r="F7" s="21" t="s">
         <v>152</v>
@@ -13018,11 +13018,11 @@
       </c>
       <c r="M7" s="37" t="str">
         <f ca="1" si="0" t="shared"/>
-        <v>12 Nov 2023</v>
+        <v>15 Nov 2023</v>
       </c>
       <c r="N7" s="37" t="str">
         <f ca="1" si="2" t="shared"/>
-        <v>20 Nov 2023</v>
+        <v>23 Nov 2023</v>
       </c>
       <c r="O7" s="21" t="s">
         <v>263</v>
@@ -13039,7 +13039,7 @@
       <c r="U7" s="44"/>
       <c r="V7" s="37" t="str">
         <f ca="1">"OP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-02-0"&amp;AutoIncrement!A2</f>
-        <v>OP-231110-02-003</v>
+        <v>OP-231113-02-004</v>
       </c>
       <c r="W7" s="19" t="s">
         <v>256</v>
@@ -13054,7 +13054,7 @@
       <c r="AE7" s="44"/>
       <c r="AF7" s="37" t="str">
         <f ca="1">'TC16-Supplier SO'!C2</f>
-        <v>sABs03-2311002</v>
+        <v>sABs04-2311002</v>
       </c>
       <c r="AG7" s="37" t="s">
         <v>81</v>
@@ -13085,15 +13085,15 @@
       </c>
       <c r="C8" s="36" t="str">
         <f ca="1"><![CDATA["o-SG-BAFCO-"&TEXT(TODAY(),"yymm")&"-"&AutoIncrement!B2&"-"&AutoIncrement!A2&"-003"]]></f>
-        <v>o-SG-BAFCO-2311-AB-03-003</v>
+        <v>o-SG-BAFCO-2311-AB-04-003</v>
       </c>
       <c r="D8" s="37" t="str">
         <f ca="1" si="1" t="shared"/>
-        <v>09 Nov 2023</v>
+        <v>12 Nov 2023</v>
       </c>
       <c r="E8" s="37" t="str">
         <f ca="1">"B-"&amp;TEXT(TODAY(),"yymm")&amp;"-"&amp;AutoIncrement!B2&amp; "-02-0"&amp;AutoIncrement!A2</f>
-        <v>B-2311-AB-02-003</v>
+        <v>B-2311-AB-02-004</v>
       </c>
       <c r="F8" s="21" t="s">
         <v>268</v>
@@ -13118,11 +13118,11 @@
       </c>
       <c r="M8" s="37" t="str">
         <f ca="1" si="0" t="shared"/>
-        <v>12 Nov 2023</v>
+        <v>15 Nov 2023</v>
       </c>
       <c r="N8" s="37" t="str">
         <f ca="1" si="2" t="shared"/>
-        <v>20 Nov 2023</v>
+        <v>23 Nov 2023</v>
       </c>
       <c r="O8" s="21" t="s">
         <v>265</v>
@@ -13147,7 +13147,7 @@
       </c>
       <c r="V8" s="37" t="str">
         <f ca="1">"OP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-03-0"&amp;AutoIncrement!A2</f>
-        <v>OP-231110-03-003</v>
+        <v>OP-231113-03-004</v>
       </c>
       <c r="W8" s="19" t="s">
         <v>256</v>
@@ -13163,7 +13163,7 @@
       </c>
       <c r="AA8" s="37" t="str">
         <f ca="1">"IP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>IP-231110-01-003</v>
+        <v>IP-231113-01-004</v>
       </c>
       <c r="AB8" s="45" t="s">
         <v>257</v>
@@ -13179,7 +13179,7 @@
       </c>
       <c r="AF8" s="37" t="str">
         <f ca="1">'TC16-Supplier SO'!C2</f>
-        <v>sABs03-2311002</v>
+        <v>sABs04-2311002</v>
       </c>
       <c r="AG8" s="37" t="s">
         <v>81</v>
@@ -13210,15 +13210,15 @@
       </c>
       <c r="C9" s="36" t="str">
         <f ca="1"><![CDATA["o-SG-BAFCO-"&TEXT(TODAY(),"yymm")&"-"&AutoIncrement!B2&"-"&AutoIncrement!A2&"-004"]]></f>
-        <v>o-SG-BAFCO-2311-AB-03-004</v>
+        <v>o-SG-BAFCO-2311-AB-04-004</v>
       </c>
       <c r="D9" s="37" t="str">
         <f ca="1" si="1" t="shared"/>
-        <v>09 Nov 2023</v>
+        <v>12 Nov 2023</v>
       </c>
       <c r="E9" s="37" t="str">
         <f ca="1">"B-"&amp;TEXT(TODAY(),"yymm")&amp;"-"&amp;AutoIncrement!B2&amp; "-03-0"&amp;AutoIncrement!A2</f>
-        <v>B-2311-AB-03-003</v>
+        <v>B-2311-AB-03-004</v>
       </c>
       <c r="F9" s="21" t="s">
         <v>268</v>
@@ -13243,11 +13243,11 @@
       </c>
       <c r="M9" s="37" t="str">
         <f ca="1" si="0" t="shared"/>
-        <v>12 Nov 2023</v>
+        <v>15 Nov 2023</v>
       </c>
       <c r="N9" s="37" t="str">
         <f ca="1" si="2" t="shared"/>
-        <v>20 Nov 2023</v>
+        <v>23 Nov 2023</v>
       </c>
       <c r="O9" s="19"/>
       <c r="P9" s="19"/>
@@ -13258,7 +13258,7 @@
       <c r="U9" s="44"/>
       <c r="V9" s="37" t="str">
         <f ca="1">"OP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-03-0"&amp;AutoIncrement!A2</f>
-        <v>OP-231110-03-003</v>
+        <v>OP-231113-03-004</v>
       </c>
       <c r="W9" s="19" t="s">
         <v>256</v>
@@ -13274,7 +13274,7 @@
       </c>
       <c r="AA9" s="37" t="str">
         <f ca="1">"IP-"&amp;TEXT(TODAY(),"yymmdd")&amp; "-01-0"&amp;AutoIncrement!A2</f>
-        <v>IP-231110-01-003</v>
+        <v>IP-231113-01-004</v>
       </c>
       <c r="AB9" s="45" t="s">
         <v>257</v>
@@ -13290,7 +13290,7 @@
       </c>
       <c r="AF9" s="37" t="str">
         <f ca="1">'TC16-Supplier SO'!C2</f>
-        <v>sABs03-2311002</v>
+        <v>sABs04-2311002</v>
       </c>
       <c r="AG9" s="37" t="s">
         <v>81</v>
@@ -13349,10 +13349,10 @@
       </c>
       <c r="B2" s="12" t="str">
         <f ca="1">'TC44-Supplier Outbound -Regular'!A3</f>
-        <v>o-SG-BAFCO-2311-AB-03-001</v>
+        <v>o-SG-BAFCO-2311-AB-04-001</v>
       </c>
       <c r="C2" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -13361,10 +13361,10 @@
       </c>
       <c r="B3" s="12" t="str">
         <f ca="1">'TC44-Supplier Outbound -Spot'!C2</f>
-        <v>o-SG-BAFCO-2311-AB-03-002</v>
+        <v>o-SG-BAFCO-2311-AB-04-002</v>
       </c>
       <c r="C3" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -13373,10 +13373,10 @@
       </c>
       <c r="B4" s="12" t="str">
         <f ca="1">'TC44-Supplier Outbound -Spot'!C6</f>
-        <v>o-SG-BAFCO-2311-AB-03-003</v>
+        <v>o-SG-BAFCO-2311-AB-04-003</v>
       </c>
       <c r="C4" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -13385,10 +13385,10 @@
       </c>
       <c r="B5" s="12" t="str">
         <f ca="1">'TC44-Supplier Outbound -Spot'!C9</f>
-        <v>o-SG-BAFCO-2311-AB-03-004</v>
+        <v>o-SG-BAFCO-2311-AB-04-004</v>
       </c>
       <c r="C5" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
   </sheetData>
@@ -13819,7 +13819,7 @@
         <v>o-SG-BAFCO-231108009</v>
       </c>
       <c r="C2" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>464</v>
@@ -13834,7 +13834,7 @@
         <v>o-SG-BAFCO-231108010</v>
       </c>
       <c r="C3" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>465</v>
@@ -13849,7 +13849,7 @@
         <v>o-SG-BAFCO-231108011</v>
       </c>
       <c r="C4" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -13861,12 +13861,12 @@
         <v>o-SG-BAFCO-231108012</v>
       </c>
       <c r="C5" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>466</v>
@@ -13975,7 +13975,7 @@
     <row customFormat="1" r="2" s="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" s="48" t="str">
         <f ca="1">'TC44-Supplier Outbound -Regular'!C3</f>
-        <v>B-2311-AB-01-003</v>
+        <v>B-2311-AB-01-004</v>
       </c>
       <c r="B2" s="48"/>
       <c r="C2" s="48" t="s">
@@ -14054,7 +14054,7 @@
     <row customFormat="1" r="3" s="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="48" t="str">
         <f ca="1">'TC44-Supplier Outbound -Regular'!C3</f>
-        <v>B-2311-AB-01-003</v>
+        <v>B-2311-AB-01-004</v>
       </c>
       <c r="B3" s="53" t="str">
         <f>'TC44-Supplier Outbound -Regular'!G4</f>
@@ -14136,7 +14136,7 @@
     <row customFormat="1" r="4" s="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="48" t="str">
         <f ca="1">'TC44-Supplier Outbound -Regular'!C3</f>
-        <v>B-2311-AB-01-003</v>
+        <v>B-2311-AB-01-004</v>
       </c>
       <c r="B4" s="53" t="str">
         <f>'TC44-Supplier Outbound -Regular'!G5</f>
@@ -14218,7 +14218,7 @@
     <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="48" t="str">
         <f ca="1">'TC44-Supplier Outbound -Regular'!C3</f>
-        <v>B-2311-AB-01-003</v>
+        <v>B-2311-AB-01-004</v>
       </c>
       <c r="B5" s="53" t="str">
         <f>'TC44-Supplier Outbound -Regular'!G7</f>
@@ -14400,7 +14400,7 @@
     <row customFormat="1" r="2" s="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" s="48" t="str">
         <f ca="1">'TC44-Supplier Outbound -Spot'!E6</f>
-        <v>B-2311-AB-02-003</v>
+        <v>B-2311-AB-02-004</v>
       </c>
       <c r="B2" s="53" t="str">
         <f>'TC44-Supplier Outbound -Spot'!O8</f>
@@ -14561,7 +14561,7 @@
     <row customFormat="1" r="4" s="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="48" t="str">
         <f ca="1">'TC44-Supplier Outbound -Spot'!E7</f>
-        <v>B-2311-AB-02-003</v>
+        <v>B-2311-AB-02-004</v>
       </c>
       <c r="B4" s="53" t="str">
         <f>'TC44-Supplier Outbound -Spot'!O6</f>
@@ -14643,7 +14643,7 @@
     <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="48" t="str">
         <f ca="1">'TC44-Supplier Outbound -Spot'!E9</f>
-        <v>B-2311-AB-03-003</v>
+        <v>B-2311-AB-03-004</v>
       </c>
       <c r="B5" s="12"/>
       <c r="C5" s="48" t="s">
@@ -14829,14 +14829,14 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="str">
         <f ca="1">'TC44-Supplier Outbound -Regular'!C3</f>
-        <v>B-2311-AB-01-003</v>
+        <v>B-2311-AB-01-004</v>
       </c>
       <c r="B2" s="12"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="str">
         <f ca="1">'TC44-Supplier Outbound -Regular'!C8</f>
-        <v>B-2311-AB-01-003</v>
+        <v>B-2311-AB-01-004</v>
       </c>
       <c r="B3" s="24" t="str">
         <f>'TC44-Supplier Outbound -Regular'!G8</f>
@@ -14846,7 +14846,7 @@
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="str">
         <f ca="1">'TC44-Supplier Outbound -Regular'!C4</f>
-        <v>B-2311-AB-01-003</v>
+        <v>B-2311-AB-01-004</v>
       </c>
       <c r="B4" s="49" t="str">
         <f>'TC44-Supplier Outbound -Regular'!G4</f>
@@ -14856,7 +14856,7 @@
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="str">
         <f ca="1">'TC44-Supplier Outbound -Regular'!C6</f>
-        <v>B-2311-AB-01-003</v>
+        <v>B-2311-AB-01-004</v>
       </c>
       <c r="B5" s="49" t="str">
         <f>'TC44-Supplier Outbound -Regular'!G6</f>
@@ -14880,7 +14880,7 @@
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="str">
         <f ca="1">'TC44-Supplier Outbound -Spot'!E8</f>
-        <v>B-2311-AB-02-003</v>
+        <v>B-2311-AB-02-004</v>
       </c>
       <c r="B8" s="24" t="str">
         <f>'TC44-Supplier Outbound -Spot'!O8</f>
@@ -14890,7 +14890,7 @@
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="str">
         <f ca="1">'TC44-Supplier Outbound -Spot'!E7</f>
-        <v>B-2311-AB-02-003</v>
+        <v>B-2311-AB-02-004</v>
       </c>
       <c r="B9" s="24" t="str">
         <f>'TC44-Supplier Outbound -Spot'!O7</f>
@@ -14900,7 +14900,7 @@
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="str">
         <f ca="1">'TC44-Supplier Outbound -Spot'!E9</f>
-        <v>B-2311-AB-03-003</v>
+        <v>B-2311-AB-03-004</v>
       </c>
       <c r="B10" s="12"/>
     </row>
@@ -14942,7 +14942,7 @@
         <v>o-SG-BAFCO-231108009</v>
       </c>
       <c r="C2" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -14954,7 +14954,7 @@
         <v>o-SG-BAFCO-231108010</v>
       </c>
       <c r="C3" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -14966,7 +14966,7 @@
         <v>o-SG-BAFCO-231108011</v>
       </c>
       <c r="C4" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -14978,7 +14978,7 @@
         <v>o-SG-BAFCO-231108012</v>
       </c>
       <c r="C5" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
   </sheetData>
@@ -15026,11 +15026,11 @@
       </c>
       <c r="B2" s="12" t="str">
         <f ca="1"><![CDATA["i-VN-AKIRA-"&TEXT(TODAY(),"yymmdd")&"-"&AutoIncrement!B2&"-"&AutoIncrement!A2&"-001"]]></f>
-        <v>i-VN-AKIRA-231110-AB-03-001</v>
+        <v>i-VN-AKIRA-231113-AB-04-001</v>
       </c>
       <c r="C2" s="37" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY()), DAY(TODAY())), "dd MMM yyyy")</f>
-        <v>10 Nov 2023</v>
+        <v>13 Nov 2023</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
@@ -15042,11 +15042,11 @@
       </c>
       <c r="B3" s="12" t="str">
         <f ca="1"><![CDATA["i-VN-AKIRA-"&TEXT(TODAY(),"yymmdd")&"-"&AutoIncrement!B2&"-"&AutoIncrement!A2&"-001"]]></f>
-        <v>i-VN-AKIRA-231110-AB-03-001</v>
+        <v>i-VN-AKIRA-231113-AB-04-001</v>
       </c>
       <c r="C3" s="37" t="str">
         <f ca="1" ref="C3:C15" si="0" t="shared">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY()), DAY(TODAY())), "dd MMM yyyy")</f>
-        <v>10 Nov 2023</v>
+        <v>13 Nov 2023</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
@@ -15058,11 +15058,11 @@
       </c>
       <c r="B4" s="12" t="str">
         <f ca="1"><![CDATA["i-VN-AKIRA-"&TEXT(TODAY(),"yymmdd")&"-"&AutoIncrement!B2&"-"&AutoIncrement!A2&"-001"]]></f>
-        <v>i-VN-AKIRA-231110-AB-03-001</v>
+        <v>i-VN-AKIRA-231113-AB-04-001</v>
       </c>
       <c r="C4" s="37" t="str">
         <f ca="1" si="0" t="shared"/>
-        <v>10 Nov 2023</v>
+        <v>13 Nov 2023</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
@@ -15074,11 +15074,11 @@
       </c>
       <c r="B5" s="12" t="str">
         <f ca="1"><![CDATA["i-VN-AKIRA-"&TEXT(TODAY(),"yymmdd")&"-"&AutoIncrement!B2&"-"&AutoIncrement!A2&"-001"]]></f>
-        <v>i-VN-AKIRA-231110-AB-03-001</v>
+        <v>i-VN-AKIRA-231113-AB-04-001</v>
       </c>
       <c r="C5" s="37" t="str">
         <f ca="1" si="0" t="shared"/>
-        <v>10 Nov 2023</v>
+        <v>13 Nov 2023</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
@@ -15090,11 +15090,11 @@
       </c>
       <c r="B6" s="12" t="str">
         <f ca="1"><![CDATA["i-VN-AKIRA-"&TEXT(TODAY(),"yymmdd")&"-"&AutoIncrement!B2&"-"&AutoIncrement!A2&"-001"]]></f>
-        <v>i-VN-AKIRA-231110-AB-03-001</v>
+        <v>i-VN-AKIRA-231113-AB-04-001</v>
       </c>
       <c r="C6" s="37" t="str">
         <f ca="1" si="0" t="shared"/>
-        <v>10 Nov 2023</v>
+        <v>13 Nov 2023</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
@@ -15106,11 +15106,11 @@
       </c>
       <c r="B7" s="12" t="str">
         <f ca="1"><![CDATA["i-VN-AKIRA-"&TEXT(TODAY(),"yymmdd")&"-"&AutoIncrement!B2&"-"&AutoIncrement!A2&"-001"]]></f>
-        <v>i-VN-AKIRA-231110-AB-03-001</v>
+        <v>i-VN-AKIRA-231113-AB-04-001</v>
       </c>
       <c r="C7" s="37" t="str">
         <f ca="1" si="0" t="shared"/>
-        <v>10 Nov 2023</v>
+        <v>13 Nov 2023</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
@@ -15122,11 +15122,11 @@
       </c>
       <c r="B8" s="12" t="str">
         <f ca="1"><![CDATA["i-VN-AKIRA-"&TEXT(TODAY(),"yymmdd")&"-"&AutoIncrement!B2&"-"&AutoIncrement!A2&"-001"]]></f>
-        <v>i-VN-AKIRA-231110-AB-03-001</v>
+        <v>i-VN-AKIRA-231113-AB-04-001</v>
       </c>
       <c r="C8" s="37" t="str">
         <f ca="1" si="0" t="shared"/>
-        <v>10 Nov 2023</v>
+        <v>13 Nov 2023</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
@@ -15138,11 +15138,11 @@
       </c>
       <c r="B9" s="12" t="str">
         <f ca="1"><![CDATA["i-VN-AKIRA-"&TEXT(TODAY(),"yymmdd")&"-"&AutoIncrement!B2&"-"&AutoIncrement!A2&"-001"]]></f>
-        <v>i-VN-AKIRA-231110-AB-03-001</v>
+        <v>i-VN-AKIRA-231113-AB-04-001</v>
       </c>
       <c r="C9" s="37" t="str">
         <f ca="1" si="0" t="shared"/>
-        <v>10 Nov 2023</v>
+        <v>13 Nov 2023</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
@@ -15154,11 +15154,11 @@
       </c>
       <c r="B10" s="12" t="str">
         <f ca="1"><![CDATA["i-VN-AKIRA-"&TEXT(TODAY(),"yymmdd")&"-"&AutoIncrement!B2&"-"&AutoIncrement!A2&"-001"]]></f>
-        <v>i-VN-AKIRA-231110-AB-03-001</v>
+        <v>i-VN-AKIRA-231113-AB-04-001</v>
       </c>
       <c r="C10" s="37" t="str">
         <f ca="1" si="0" t="shared"/>
-        <v>10 Nov 2023</v>
+        <v>13 Nov 2023</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
@@ -15170,11 +15170,11 @@
       </c>
       <c r="B11" s="12" t="str">
         <f ca="1"><![CDATA["i-VN-AKIRA-"&TEXT(TODAY(),"yymmdd")&"-"&AutoIncrement!B2&"-"&AutoIncrement!A2&"-001"]]></f>
-        <v>i-VN-AKIRA-231110-AB-03-001</v>
+        <v>i-VN-AKIRA-231113-AB-04-001</v>
       </c>
       <c r="C11" s="37" t="str">
         <f ca="1" si="0" t="shared"/>
-        <v>10 Nov 2023</v>
+        <v>13 Nov 2023</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
@@ -15186,11 +15186,11 @@
       </c>
       <c r="B12" s="12" t="str">
         <f ca="1"><![CDATA["i-VN-AKIRA-"&TEXT(TODAY(),"yymmdd")&"-"&AutoIncrement!B2&"-"&AutoIncrement!A2&"-001"]]></f>
-        <v>i-VN-AKIRA-231110-AB-03-001</v>
+        <v>i-VN-AKIRA-231113-AB-04-001</v>
       </c>
       <c r="C12" s="37" t="str">
         <f ca="1" si="0" t="shared"/>
-        <v>10 Nov 2023</v>
+        <v>13 Nov 2023</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
@@ -15202,11 +15202,11 @@
       </c>
       <c r="B13" s="12" t="str">
         <f ca="1"><![CDATA["i-VN-AKIRA-"&TEXT(TODAY(),"yymmdd")&"-"&AutoIncrement!B2&"-"&AutoIncrement!A2&"-001"]]></f>
-        <v>i-VN-AKIRA-231110-AB-03-001</v>
+        <v>i-VN-AKIRA-231113-AB-04-001</v>
       </c>
       <c r="C13" s="37" t="str">
         <f ca="1" si="0" t="shared"/>
-        <v>10 Nov 2023</v>
+        <v>13 Nov 2023</v>
       </c>
       <c r="D13" s="50">
         <v>1</v>
@@ -15224,11 +15224,11 @@
       </c>
       <c r="B14" s="12" t="str">
         <f ca="1"><![CDATA["i-VN-AKIRA-"&TEXT(TODAY(),"yymmdd")&"-"&AutoIncrement!B2&"-"&AutoIncrement!A2&"-002"]]></f>
-        <v>i-VN-AKIRA-231110-AB-03-002</v>
+        <v>i-VN-AKIRA-231113-AB-04-002</v>
       </c>
       <c r="C14" s="37" t="str">
         <f ca="1" si="0" t="shared"/>
-        <v>10 Nov 2023</v>
+        <v>13 Nov 2023</v>
       </c>
       <c r="D14" s="50">
         <v>1</v>
@@ -15246,11 +15246,11 @@
       </c>
       <c r="B15" s="12" t="str">
         <f ca="1"><![CDATA["i-VN-AKIRA-"&TEXT(TODAY(),"yymmdd")&"-"&AutoIncrement!B2&"-"&AutoIncrement!A2&"-002"]]></f>
-        <v>i-VN-AKIRA-231110-AB-03-002</v>
+        <v>i-VN-AKIRA-231113-AB-04-002</v>
       </c>
       <c r="C15" s="37" t="str">
         <f ca="1" si="0" t="shared"/>
-        <v>10 Nov 2023</v>
+        <v>13 Nov 2023</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
@@ -15407,7 +15407,7 @@
       </c>
       <c r="E2" s="12" t="str">
         <f>'TC4'!C2</f>
-        <v>SGTTAP-VNTTVN-AB-03-003</v>
+        <v>SGTTAP-VNTTVN-AB-04-004</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>411</v>
@@ -15457,7 +15457,7 @@
       </c>
       <c r="E3" s="52" t="str">
         <f>'TC4'!C2</f>
-        <v>SGTTAP-VNTTVN-AB-03-003</v>
+        <v>SGTTAP-VNTTVN-AB-04-004</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>411</v>
@@ -15507,7 +15507,7 @@
       </c>
       <c r="E4" s="52" t="str">
         <f>'TC4'!C2</f>
-        <v>SGTTAP-VNTTVN-AB-03-003</v>
+        <v>SGTTAP-VNTTVN-AB-04-004</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>412</v>
@@ -15557,7 +15557,7 @@
       </c>
       <c r="E5" s="52" t="str">
         <f>'TC4'!C2</f>
-        <v>SGTTAP-VNTTVN-AB-03-003</v>
+        <v>SGTTAP-VNTTVN-AB-04-004</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>412</v>
@@ -15606,7 +15606,7 @@
       </c>
       <c r="E6" s="52" t="str">
         <f>'TC4'!C2</f>
-        <v>SGTTAP-VNTTVN-AB-03-003</v>
+        <v>SGTTAP-VNTTVN-AB-04-004</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>413</v>
@@ -15655,7 +15655,7 @@
       </c>
       <c r="E7" s="52" t="str">
         <f>'TC4'!C2</f>
-        <v>SGTTAP-VNTTVN-AB-03-003</v>
+        <v>SGTTAP-VNTTVN-AB-04-004</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>413</v>
@@ -15792,7 +15792,7 @@
       </c>
       <c r="C2" s="20" t="str">
         <f>"SGTTAP-VNTTVN-"&amp;'TC4'!H2&amp;"-0"&amp;AutoIncrement!A2</f>
-        <v>SGTTAP-VNTTVN-AB-03-003</v>
+        <v>SGTTAP-VNTTVN-AB-04-004</v>
       </c>
       <c r="D2" s="20" t="s">
         <v>20</v>
@@ -15808,11 +15808,11 @@
       </c>
       <c r="H2" s="20" t="str">
         <f>AutoIncrement!B2&amp;"-"&amp;AutoIncrement!A2</f>
-        <v>AB-03</v>
+        <v>AB-04</v>
       </c>
       <c r="I2" s="20" t="str">
         <f>"CD-"&amp;H2</f>
-        <v>CD-AB-03</v>
+        <v>CD-AB-04</v>
       </c>
       <c r="J2" s="20" t="str">
         <f>'TC3.1'!B2&amp;"("&amp;'TC3.1'!C2&amp;")"</f>
@@ -15829,7 +15829,7 @@
       </c>
       <c r="N2" s="20" t="str">
         <f>"RD-"&amp;H2</f>
-        <v>RD-AB-03</v>
+        <v>RD-AB-04</v>
       </c>
       <c r="O2" s="20" t="s">
         <v>23</v>

</xml_diff>